<commit_message>
Add Freddo inflationary measure
</commit_message>
<xml_diff>
--- a/Pay 2007-2022.xlsx
+++ b/Pay 2007-2022.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelshaw/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77F07529-139A-394B-AB1F-93C590EE24B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAB8C29B-F4C1-CB49-B4D4-34D686DAAF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13140" yWindow="0" windowWidth="20460" windowHeight="21000" xr2:uid="{E1BF444D-A2ED-614E-ACCD-35609FC30102}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Pay" sheetId="2" r:id="rId2"/>
+    <sheet name="Pay 2007-2022" sheetId="2" r:id="rId2"/>
     <sheet name="NROC" sheetId="3" r:id="rId3"/>
     <sheet name="Inflation" sheetId="4" r:id="rId4"/>
     <sheet name="Notes" sheetId="5" r:id="rId5"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t>FY1</t>
   </si>
@@ -247,6 +247,24 @@
   </si>
   <si>
     <t>Measure</t>
+  </si>
+  <si>
+    <t>Freddo Multiplier</t>
+  </si>
+  <si>
+    <t>FY1 (2007, Freddo)</t>
+  </si>
+  <si>
+    <t>FY2 (2007, Freddo)</t>
+  </si>
+  <si>
+    <t>CT1 (2007, Freddo)</t>
+  </si>
+  <si>
+    <t>CT3 (2007, Freddo)</t>
+  </si>
+  <si>
+    <t>CT6 (2007, Freddo)</t>
   </si>
 </sst>
 </file>
@@ -681,13 +699,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3275042D-364E-CE44-842E-2AA03D01A8E4}">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomRight" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2131,1525 +2149,2344 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33">
+        <f>$B$30/B30</f>
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:Q33" si="0">$B$30/C30</f>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.88235294117647045</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>47</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <f>$B$31/B31</f>
         <v>1</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <f>$B$31/C31</f>
         <v>0.96576151121605658</v>
       </c>
-      <c r="D33">
+      <c r="D34">
         <f>$B$31/D31</f>
         <v>0.94457274826789839</v>
       </c>
-      <c r="E33">
+      <c r="E34">
         <f>$B$31/E31</f>
         <v>0.91498881431767332</v>
       </c>
-      <c r="F33">
+      <c r="F34">
         <f>$B$31/F31</f>
         <v>0.87580299785867233</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <f>$B$31/G31</f>
         <v>0.85119667013527578</v>
       </c>
-      <c r="H33">
+      <c r="H34">
         <f>$B$31/H31</f>
         <v>0.8304568527918782</v>
       </c>
-      <c r="I33">
+      <c r="I34">
         <f>$B$31/I31</f>
         <v>0.81799999999999995</v>
       </c>
-      <c r="J33">
+      <c r="J34">
         <f>$B$31/J31</f>
         <v>0.81799999999999995</v>
       </c>
-      <c r="K33">
+      <c r="K34">
         <f>$B$31/K31</f>
         <v>0.81231380337636538</v>
       </c>
-      <c r="L33">
+      <c r="L34">
         <f>$B$31/L31</f>
         <v>0.79110251450676972</v>
       </c>
-      <c r="M33">
+      <c r="M34">
         <f>$B$31/M31</f>
         <v>0.77242681775259669</v>
       </c>
-      <c r="N33">
+      <c r="N34">
         <f>$B$31/N31</f>
         <v>0.75881261595547311</v>
       </c>
-      <c r="O33">
+      <c r="O34">
         <f>$B$31/O31</f>
         <v>0.75252989880404775</v>
       </c>
-      <c r="P33">
+      <c r="P34">
         <f>$B$31/P31</f>
         <v>0.73297491039426521</v>
       </c>
-      <c r="Q33">
+      <c r="Q34">
         <f>$B$31/Q31</f>
         <v>0.67214461791290059</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>48</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <f>$B$32/B32</f>
         <v>1</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <f>$B$32/C32</f>
         <v>0.96182495344506513</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <f>$B$32/D32</f>
         <v>0.96677585400093591</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <f>$B$32/E32</f>
         <v>0.92397137745974955</v>
       </c>
-      <c r="F34">
+      <c r="F35">
         <f>$B$32/F32</f>
         <v>0.87840136054421769</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <f>$B$32/G32</f>
         <v>0.85125669550885874</v>
       </c>
-      <c r="H34">
+      <c r="H35">
         <f>$B$32/H32</f>
         <v>0.82606957217113153</v>
       </c>
-      <c r="I34">
+      <c r="I35">
         <f>$B$32/I32</f>
         <v>0.80703124999999998</v>
       </c>
-      <c r="J34">
+      <c r="J35">
         <f>$B$32/J32</f>
         <v>0.79922630560928432</v>
       </c>
-      <c r="K34">
+      <c r="K35">
         <f>$B$32/K32</f>
         <v>0.78525275560623331</v>
       </c>
-      <c r="L34">
+      <c r="L35">
         <f>$B$32/L32</f>
         <v>0.75816513761467885</v>
       </c>
-      <c r="M34">
+      <c r="M35">
         <f>$B$32/M32</f>
         <v>0.7336647727272726</v>
       </c>
-      <c r="N34">
+      <c r="N35">
         <f>$B$32/N32</f>
         <v>0.71537396121883656</v>
       </c>
-      <c r="O34">
+      <c r="O35">
         <f>$B$32/O32</f>
         <v>0.70487888092801088</v>
       </c>
-      <c r="P34">
+      <c r="P35">
         <f>$B$32/P32</f>
         <v>0.67737704918032782</v>
       </c>
-      <c r="Q34">
+      <c r="Q35">
         <f>$B$32/Q32</f>
         <v>0.6071113723185424</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>41</v>
       </c>
-      <c r="B36">
+      <c r="B37">
+        <f>(B$4*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <v>31578</v>
+      </c>
+      <c r="C37">
+        <f>(C$4*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <v>31670.217237308145</v>
+      </c>
+      <c r="D37">
+        <f>(D$4*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <v>31440.103926096999</v>
+      </c>
+      <c r="E37">
+        <f>(E$4*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <v>30760.093959731541</v>
+      </c>
+      <c r="F37">
+        <f>(F$4*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <v>29442.745182012848</v>
+      </c>
+      <c r="G37">
+        <f>(G$4*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <v>28615.529656607701</v>
+      </c>
+      <c r="H37">
+        <f>(H$4*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <v>28197.331979695431</v>
+      </c>
+      <c r="I37">
+        <f>(I$4*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <v>27774.371999999999</v>
+      </c>
+      <c r="J37">
+        <f>(J$4*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <v>27774.371999999999</v>
+      </c>
+      <c r="K37">
+        <f>(K$4*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <v>27856.677259185697</v>
+      </c>
+      <c r="L37">
+        <f>(L$4*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <v>27602.321442940032</v>
+      </c>
+      <c r="M37">
+        <f>(M$4*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <v>27489.439195467414</v>
+      </c>
+      <c r="N37">
+        <f>(N$4*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <v>27545.109667903522</v>
+      </c>
+      <c r="O37">
+        <f>(O$4*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <v>27863.603232750684</v>
+      </c>
+      <c r="P37">
+        <f>(P$4*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <v>27682.474537634407</v>
+      </c>
+      <c r="Q37">
+        <f>(Q$4*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <v>25892.63996055875</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="7">
+        <f>B37/$B37</f>
+        <v>1</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" ref="C38" si="1">C37/$B37</f>
+        <v>1.0029203001237617</v>
+      </c>
+      <c r="D38" s="7">
+        <f t="shared" ref="D38" si="2">D37/$B37</f>
+        <v>0.99563315998787127</v>
+      </c>
+      <c r="E38" s="7">
+        <f t="shared" ref="E38" si="3">E37/$B37</f>
+        <v>0.97409886502411613</v>
+      </c>
+      <c r="F38" s="7">
+        <f t="shared" ref="F38" si="4">F37/$B37</f>
+        <v>0.93238156887747314</v>
+      </c>
+      <c r="G38" s="7">
+        <f t="shared" ref="G38" si="5">G37/$B37</f>
+        <v>0.90618562469465136</v>
+      </c>
+      <c r="H38" s="7">
+        <f t="shared" ref="H38" si="6">H37/$B37</f>
+        <v>0.89294230095938409</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" ref="I38" si="7">I37/$B37</f>
+        <v>0.87954816644499334</v>
+      </c>
+      <c r="J38" s="7">
+        <f t="shared" ref="J38" si="8">J37/$B37</f>
+        <v>0.87954816644499334</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" ref="K38" si="9">K37/$B37</f>
+        <v>0.88215457784488238</v>
+      </c>
+      <c r="L38" s="7">
+        <f t="shared" ref="L38" si="10">L37/$B37</f>
+        <v>0.87409973535182828</v>
+      </c>
+      <c r="M38" s="7">
+        <f t="shared" ref="M38" si="11">M37/$B37</f>
+        <v>0.87052502360717632</v>
+      </c>
+      <c r="N38" s="7">
+        <f t="shared" ref="N38" si="12">N37/$B37</f>
+        <v>0.87228797478952191</v>
+      </c>
+      <c r="O38" s="7">
+        <f t="shared" ref="O38" si="13">O37/$B37</f>
+        <v>0.88237390692097928</v>
+      </c>
+      <c r="P38" s="7">
+        <f t="shared" ref="P38" si="14">P37/$B37</f>
+        <v>0.8766379928315412</v>
+      </c>
+      <c r="Q38" s="7">
+        <f t="shared" ref="Q38" si="15">Q37/$B37</f>
+        <v>0.81995819749695198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <f>(B$5*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <v>39405</v>
+      </c>
+      <c r="C39">
+        <f>(C$5*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <v>39281.383707201887</v>
+      </c>
+      <c r="D39">
+        <f>(D$5*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <v>38996.213625866054</v>
+      </c>
+      <c r="E39">
+        <f>(E$5*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <v>38152.288590604025</v>
+      </c>
+      <c r="F39">
+        <f>(F$5*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <v>36518.357601713062</v>
+      </c>
+      <c r="G39">
+        <f>(G$5*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <v>35492.347554630593</v>
+      </c>
+      <c r="H39">
+        <f>(H$5*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <v>34973.85989847716</v>
+      </c>
+      <c r="I39">
+        <f>(I$5*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <v>34449.252</v>
+      </c>
+      <c r="J39">
+        <f>(J$5*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <v>34449.252</v>
+      </c>
+      <c r="K39">
+        <f>(K$5*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <v>34552.173783515391</v>
+      </c>
+      <c r="L39">
+        <f>(L$5*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <v>31948.95588974854</v>
+      </c>
+      <c r="M39">
+        <f>(M$5*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <v>31819.537257790362</v>
+      </c>
+      <c r="N39">
+        <f>(N$5*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <v>31883.447031539887</v>
+      </c>
+      <c r="O39">
+        <f>(O$5*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <v>32251.851902483897</v>
+      </c>
+      <c r="P39">
+        <f>(P$5*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <v>32042.214435483867</v>
+      </c>
+      <c r="Q39">
+        <f>(Q$5*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <v>29970.748377978634</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="7">
+        <f>B39/$B39</f>
+        <v>1</v>
+      </c>
+      <c r="C40" s="7">
+        <f t="shared" ref="C40" si="16">C39/$B39</f>
+        <v>0.99686292874513105</v>
+      </c>
+      <c r="D40" s="7">
+        <f t="shared" ref="D40" si="17">D39/$B39</f>
+        <v>0.98962602781033004</v>
+      </c>
+      <c r="E40" s="7">
+        <f t="shared" ref="E40" si="18">E39/$B39</f>
+        <v>0.96820932852693886</v>
+      </c>
+      <c r="F40" s="7">
+        <f t="shared" ref="F40" si="19">F39/$B39</f>
+        <v>0.92674426092407214</v>
+      </c>
+      <c r="G40" s="7">
+        <f t="shared" ref="G40" si="20">G39/$B39</f>
+        <v>0.90070670104379125</v>
+      </c>
+      <c r="H40" s="7">
+        <f t="shared" ref="H40" si="21">H39/$B39</f>
+        <v>0.88754878564844963</v>
+      </c>
+      <c r="I40" s="7">
+        <f t="shared" ref="I40" si="22">I39/$B39</f>
+        <v>0.87423555386372287</v>
+      </c>
+      <c r="J40" s="7">
+        <f t="shared" ref="J40" si="23">J39/$B39</f>
+        <v>0.87423555386372287</v>
+      </c>
+      <c r="K40" s="7">
+        <f t="shared" ref="K40" si="24">K39/$B39</f>
+        <v>0.87684745041277479</v>
+      </c>
+      <c r="L40" s="7">
+        <f t="shared" ref="L40" si="25">L39/$B39</f>
+        <v>0.81078431391317196</v>
+      </c>
+      <c r="M40" s="7">
+        <f t="shared" ref="M40" si="26">M39/$B39</f>
+        <v>0.80749999385332727</v>
+      </c>
+      <c r="N40" s="7">
+        <f t="shared" ref="N40" si="27">N39/$B39</f>
+        <v>0.80912186350818138</v>
+      </c>
+      <c r="O40" s="7">
+        <f t="shared" ref="O40" si="28">O39/$B39</f>
+        <v>0.81847105449775148</v>
+      </c>
+      <c r="P40" s="7">
+        <f t="shared" ref="P40" si="29">P39/$B39</f>
+        <v>0.81315098174048639</v>
+      </c>
+      <c r="Q40" s="7">
+        <f t="shared" ref="Q40" si="30">Q39/$B39</f>
+        <v>0.76058237223648351</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41">
+        <f>(B$6*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <v>42177</v>
+      </c>
+      <c r="C41">
+        <f>(C$6*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <v>41975.858323494685</v>
+      </c>
+      <c r="D41">
+        <f>(D$6*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <v>41671.243648960743</v>
+      </c>
+      <c r="E41">
+        <f>(E$6*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <v>40769.614093959732</v>
+      </c>
+      <c r="F41">
+        <f>(F$6*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <v>39023.592077087793</v>
+      </c>
+      <c r="G41">
+        <f>(G$6*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <v>37927.195629552552</v>
+      </c>
+      <c r="H41">
+        <f>(H$6*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <v>37373.049746192897</v>
+      </c>
+      <c r="I41">
+        <f>(I$6*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <v>36812.453999999998</v>
+      </c>
+      <c r="J41">
+        <f>(J$6*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <v>36812.453999999998</v>
+      </c>
+      <c r="K41">
+        <f>(K$6*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <v>36922.099304865937</v>
+      </c>
+      <c r="L41">
+        <f>(L$6*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <v>37814.993692456475</v>
+      </c>
+      <c r="M41">
+        <f>(M$6*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <v>37661.524096317276</v>
+      </c>
+      <c r="N41">
+        <f>(N$6*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <v>37737.864684601111</v>
+      </c>
+      <c r="O41">
+        <f>(O$6*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <v>38174.211786568529</v>
+      </c>
+      <c r="P41">
+        <f>(P$6*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <v>37925.028553763441</v>
+      </c>
+      <c r="Q41">
+        <f>(Q$6*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <v>35473.727433032043</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="7">
+        <f>B41/$B41</f>
+        <v>1</v>
+      </c>
+      <c r="C42" s="7">
+        <f t="shared" ref="C42:Q42" si="31">C41/$B41</f>
+        <v>0.99523101034911643</v>
+      </c>
+      <c r="D42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.98800871681155</v>
+      </c>
+      <c r="E42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.9666314364217401</v>
+      </c>
+      <c r="F42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.92523394449789675</v>
+      </c>
+      <c r="G42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.89923881806559391</v>
+      </c>
+      <c r="H42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.88610023819126293</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.87280873461839381</v>
+      </c>
+      <c r="J42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.87280873461839381</v>
+      </c>
+      <c r="K42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.87540838146065236</v>
+      </c>
+      <c r="L42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.89657855448363977</v>
+      </c>
+      <c r="M42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.89293985101636619</v>
+      </c>
+      <c r="N42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.89474985619178959</v>
+      </c>
+      <c r="O42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.90509547351799624</v>
+      </c>
+      <c r="P42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.89918743755514718</v>
+      </c>
+      <c r="Q42" s="7">
+        <f t="shared" si="31"/>
+        <v>0.84106805683268238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43">
+        <f>(B$8*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <v>48507</v>
+      </c>
+      <c r="C43">
+        <f>(C$8*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <v>48132.587957497046</v>
+      </c>
+      <c r="D43">
+        <f>(D$8*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <v>47782.15704387991</v>
+      </c>
+      <c r="E43">
+        <f>(E$8*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <v>46748.151006711407</v>
+      </c>
+      <c r="F43">
+        <f>(F$8*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <v>44746.088865096361</v>
+      </c>
+      <c r="G43">
+        <f>(G$8*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <v>43488.914672216444</v>
+      </c>
+      <c r="H43">
+        <f>(H$8*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <v>42854.064974619294</v>
+      </c>
+      <c r="I43">
+        <f>(I$8*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <v>42211.254000000001</v>
+      </c>
+      <c r="J43">
+        <f>(J$8*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <v>42211.254000000001</v>
+      </c>
+      <c r="K43">
+        <f>(K$8*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <v>42336.983118172786</v>
+      </c>
+      <c r="L43">
+        <f>(L$8*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <v>47923.952402321069</v>
+      </c>
+      <c r="M43">
+        <f>(M$8*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <v>47728.293235127472</v>
+      </c>
+      <c r="N43">
+        <f>(N$8*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <v>47825.170547309834</v>
+      </c>
+      <c r="O43">
+        <f>(O$8*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <v>48377.284570377175</v>
+      </c>
+      <c r="P43">
+        <f>(P$8*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <v>48062.841188172039</v>
+      </c>
+      <c r="Q43">
+        <f>(Q$8*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <v>44955.241385373869</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7">
+        <f>B43/$B43</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="7">
+        <f t="shared" ref="C44:Q44" si="32">C43/$B43</f>
+        <v>0.992281278114438</v>
+      </c>
+      <c r="D44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.98505694114003983</v>
+      </c>
+      <c r="E44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.96374030566127378</v>
+      </c>
+      <c r="F44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.92246663090061976</v>
+      </c>
+      <c r="G44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.89654925417396347</v>
+      </c>
+      <c r="H44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.88346145864760328</v>
+      </c>
+      <c r="I44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.87020953676788915</v>
+      </c>
+      <c r="J44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.87020953676788915</v>
+      </c>
+      <c r="K44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.87280151561986485</v>
+      </c>
+      <c r="L44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.98798013487375158</v>
+      </c>
+      <c r="M44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.98394650741392942</v>
+      </c>
+      <c r="N44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.98594368951511813</v>
+      </c>
+      <c r="O44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.997325841020413</v>
+      </c>
+      <c r="P44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.99084340792405301</v>
+      </c>
+      <c r="Q44" s="7">
+        <f t="shared" si="32"/>
+        <v>0.9267784316773634</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45">
+        <f>(B$11*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <v>56119.5</v>
+      </c>
+      <c r="C45">
+        <f>(C$11*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <v>55535.14994096812</v>
+      </c>
+      <c r="D45">
+        <f>(D$11*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <v>55131.40531177829</v>
+      </c>
+      <c r="E45">
+        <f>(E$11*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <v>53938.590604026846</v>
+      </c>
+      <c r="F45">
+        <f>(F$11*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <v>51628.586723768734</v>
+      </c>
+      <c r="G45">
+        <f>(G$11*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <v>50178.043704474505</v>
+      </c>
+      <c r="H45">
+        <f>(H$11*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <v>49444.985786802034</v>
+      </c>
+      <c r="I45">
+        <f>(I$11*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <v>48703.310999999994</v>
+      </c>
+      <c r="J45">
+        <f>(J$11*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <v>48703.310999999994</v>
+      </c>
+      <c r="K45">
+        <f>(K$11*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <v>48848.490566037734</v>
+      </c>
+      <c r="L45">
+        <f>(L$11*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <v>47923.952402321069</v>
+      </c>
+      <c r="M45">
+        <f>(M$11*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <v>47728.293235127472</v>
+      </c>
+      <c r="N45">
+        <f>(N$11*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <v>47825.170547309834</v>
+      </c>
+      <c r="O45">
+        <f>(O$11*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <v>48377.284570377175</v>
+      </c>
+      <c r="P45">
+        <f>(P$11*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <v>51003.287317204296</v>
+      </c>
+      <c r="Q45">
+        <f>(Q$11*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <v>51459.242731306484</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="7">
+        <f>B45/$B45</f>
+        <v>1</v>
+      </c>
+      <c r="C46" s="7">
+        <f t="shared" ref="C46:Q46" si="33">C45/$B45</f>
+        <v>0.98958739726776113</v>
+      </c>
+      <c r="D46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.98239302402513007</v>
+      </c>
+      <c r="E46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.9611381178383066</v>
+      </c>
+      <c r="F46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.91997588581097001</v>
+      </c>
+      <c r="G46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.89412848839484504</v>
+      </c>
+      <c r="H46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.88106604276235589</v>
+      </c>
+      <c r="I46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.86785005212092048</v>
+      </c>
+      <c r="J46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.86785005212092048</v>
+      </c>
+      <c r="K46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.87043702395847666</v>
+      </c>
+      <c r="L46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.85396256920181168</v>
+      </c>
+      <c r="M46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.85047609538801083</v>
+      </c>
+      <c r="N46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.85220236365808377</v>
+      </c>
+      <c r="O46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.86204054865736823</v>
+      </c>
+      <c r="P46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.90883360181762662</v>
+      </c>
+      <c r="Q46" s="7">
+        <f t="shared" si="33"/>
+        <v>0.91695832520436715</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48">
+        <f>(B$4*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <v>31578</v>
+      </c>
+      <c r="C48">
+        <f>(C$4*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <v>31541.12569832402</v>
+      </c>
+      <c r="D48">
+        <f>(D$4*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <v>32179.134300421152</v>
+      </c>
+      <c r="E48">
+        <f>(E$4*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <v>31062.069767441859</v>
+      </c>
+      <c r="F48">
+        <f>(F$4*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <v>29530.09693877551</v>
+      </c>
+      <c r="G48">
+        <f>(G$4*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <v>28617.547589616814</v>
+      </c>
+      <c r="H48">
+        <f>(H$4*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <v>28048.3662534986</v>
+      </c>
+      <c r="I48">
+        <f>(I$4*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <v>27401.939062499998</v>
+      </c>
+      <c r="J48">
+        <f>(J$4*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <v>27136.929980657638</v>
+      </c>
+      <c r="K48">
+        <f>(K$4*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <v>26928.672748004559</v>
+      </c>
+      <c r="L48">
+        <f>(L$4*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <v>26453.104940917427</v>
+      </c>
+      <c r="M48">
+        <f>(M$4*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <v>26109.9597997159</v>
+      </c>
+      <c r="N48">
+        <f>(N$4*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <v>25968.274381578944</v>
+      </c>
+      <c r="O48">
+        <f>(O$4*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <v>26099.249340839298</v>
+      </c>
+      <c r="P48">
+        <f>(P$4*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <v>25582.694100983605</v>
+      </c>
+      <c r="Q48">
+        <f>(Q$4*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <v>23387.401699676753</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="7">
+        <f t="shared" ref="B49" si="34">B48/$B48</f>
+        <v>1</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="shared" ref="C49" si="35">C48/$B48</f>
+        <v>0.99883227874862313</v>
+      </c>
+      <c r="D49" s="7">
+        <f t="shared" ref="D49" si="36">D48/$B48</f>
+        <v>1.0190364906080547</v>
+      </c>
+      <c r="E49" s="7">
+        <f t="shared" ref="E49" si="37">E48/$B48</f>
+        <v>0.9836617191539001</v>
+      </c>
+      <c r="F49" s="7">
+        <f t="shared" ref="F49" si="38">F48/$B48</f>
+        <v>0.9351477908282827</v>
+      </c>
+      <c r="G49" s="7">
+        <f t="shared" ref="G49" si="39">G48/$B48</f>
+        <v>0.9062495278237005</v>
+      </c>
+      <c r="H49" s="7">
+        <f t="shared" ref="H49" si="40">H48/$B48</f>
+        <v>0.88822491144146554</v>
+      </c>
+      <c r="I49" s="7">
+        <f t="shared" ref="I49" si="41">I48/$B48</f>
+        <v>0.86775410293558797</v>
+      </c>
+      <c r="J49" s="7">
+        <f t="shared" ref="J49" si="42">J48/$B48</f>
+        <v>0.8593618969110659</v>
+      </c>
+      <c r="K49" s="7">
+        <f t="shared" ref="K49" si="43">K48/$B48</f>
+        <v>0.85276688669341183</v>
+      </c>
+      <c r="L49" s="7">
+        <f t="shared" ref="L49" si="44">L48/$B48</f>
+        <v>0.83770678766601514</v>
+      </c>
+      <c r="M49" s="7">
+        <f t="shared" ref="M49" si="45">M48/$B48</f>
+        <v>0.82684019886363602</v>
+      </c>
+      <c r="N49" s="7">
+        <f t="shared" ref="N49" si="46">N48/$B48</f>
+        <v>0.82235335935078036</v>
+      </c>
+      <c r="O49" s="7">
+        <f t="shared" ref="O49" si="47">O48/$B48</f>
+        <v>0.82650102415730253</v>
+      </c>
+      <c r="P49" s="7">
+        <f t="shared" ref="P49" si="48">P48/$B48</f>
+        <v>0.81014295081967203</v>
+      </c>
+      <c r="Q49" s="7">
+        <f t="shared" ref="Q49" si="49">Q48/$B48</f>
+        <v>0.7406232725212728</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50">
+        <f>(B$5*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <v>39405</v>
+      </c>
+      <c r="C50">
+        <f>(C$5*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <v>39121.26815642458</v>
+      </c>
+      <c r="D50">
+        <f>(D$5*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <v>39912.857744501642</v>
+      </c>
+      <c r="E50">
+        <f>(E$5*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <v>38526.834525939179</v>
+      </c>
+      <c r="F50">
+        <f>(F$5*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <v>36626.701530612248</v>
+      </c>
+      <c r="G50">
+        <f>(G$5*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <v>35494.850432632884</v>
+      </c>
+      <c r="H50">
+        <f>(H$5*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <v>34789.093962415034</v>
+      </c>
+      <c r="I50">
+        <f>(I$5*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <v>33987.314062500001</v>
+      </c>
+      <c r="J50">
+        <f>(J$5*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <v>33658.616634429396</v>
+      </c>
+      <c r="K50">
+        <f>(K$5*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <v>33401.118586088938</v>
+      </c>
+      <c r="L50">
+        <f>(L$5*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <v>30618.768231192655</v>
+      </c>
+      <c r="M50">
+        <f>(M$5*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <v>30222.764194602267</v>
+      </c>
+      <c r="N50">
+        <f>(N$5*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <v>30058.261184210522</v>
+      </c>
+      <c r="O50">
+        <f>(O$5*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <v>30209.629295803476</v>
+      </c>
+      <c r="P50">
+        <f>(P$5*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <v>29611.737531147537</v>
+      </c>
+      <c r="Q50">
+        <f>(Q$5*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <v>27070.933385836022</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" s="7">
+        <f t="shared" ref="B51" si="50">B50/$B50</f>
+        <v>1</v>
+      </c>
+      <c r="C51" s="7">
+        <f t="shared" ref="C51" si="51">C50/$B50</f>
+        <v>0.99279959792982053</v>
+      </c>
+      <c r="D51" s="7">
+        <f t="shared" ref="D51" si="52">D50/$B50</f>
+        <v>1.0128881549169304</v>
+      </c>
+      <c r="E51" s="7">
+        <f t="shared" ref="E51" si="53">E50/$B50</f>
+        <v>0.97771436431770531</v>
+      </c>
+      <c r="F51" s="7">
+        <f t="shared" ref="F51" si="54">F50/$B50</f>
+        <v>0.92949375791428113</v>
+      </c>
+      <c r="G51" s="7">
+        <f t="shared" ref="G51" si="55">G50/$B50</f>
+        <v>0.90077021780568156</v>
+      </c>
+      <c r="H51" s="7">
+        <f t="shared" ref="H51" si="56">H50/$B50</f>
+        <v>0.88285988992298015</v>
+      </c>
+      <c r="I51" s="7">
+        <f t="shared" ref="I51" si="57">I50/$B50</f>
+        <v>0.86251272839741155</v>
+      </c>
+      <c r="J51" s="7">
+        <f t="shared" ref="J51" si="58">J50/$B50</f>
+        <v>0.85417121264888707</v>
+      </c>
+      <c r="K51" s="7">
+        <f t="shared" ref="K51" si="59">K50/$B50</f>
+        <v>0.84763655845930563</v>
+      </c>
+      <c r="L51" s="7">
+        <f t="shared" ref="L51" si="60">L50/$B50</f>
+        <v>0.77702748968893931</v>
+      </c>
+      <c r="M51" s="7">
+        <f t="shared" ref="M51" si="61">M50/$B50</f>
+        <v>0.76697790114458231</v>
+      </c>
+      <c r="N51" s="7">
+        <f t="shared" ref="N51" si="62">N50/$B50</f>
+        <v>0.76280322761605179</v>
+      </c>
+      <c r="O51" s="7">
+        <f t="shared" ref="O51" si="63">O50/$B50</f>
+        <v>0.76664457037948164</v>
+      </c>
+      <c r="P51" s="7">
+        <f t="shared" ref="P51" si="64">P50/$B50</f>
+        <v>0.75147157800146014</v>
+      </c>
+      <c r="Q51" s="7">
+        <f t="shared" ref="Q51" si="65">Q50/$B50</f>
+        <v>0.68699234578951962</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52">
+        <f>(B$6*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <v>42177</v>
+      </c>
+      <c r="C52">
+        <f>(C$6*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <v>41804.75977653631</v>
+      </c>
+      <c r="D52">
+        <f>(D$6*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <v>42650.766963032293</v>
+      </c>
+      <c r="E52">
+        <f>(E$6*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <v>41169.854651162794</v>
+      </c>
+      <c r="F52">
+        <f>(F$6*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <v>39139.368622448979</v>
+      </c>
+      <c r="G52">
+        <f>(G$6*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <v>37929.870210135974</v>
+      </c>
+      <c r="H52">
+        <f>(H$6*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <v>37175.608956417433</v>
+      </c>
+      <c r="I52">
+        <f>(I$6*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <v>36318.827343749996</v>
+      </c>
+      <c r="J52">
+        <f>(J$6*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <v>35967.58143133462</v>
+      </c>
+      <c r="K52">
+        <f>(K$6*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <v>35692.093500570125</v>
+      </c>
+      <c r="L52">
+        <f>(L$6*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <v>36240.574857247702</v>
+      </c>
+      <c r="M52">
+        <f>(M$6*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <v>35771.587523437491</v>
+      </c>
+      <c r="N52">
+        <f>(N$6*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <v>35577.539407894736</v>
+      </c>
+      <c r="O52">
+        <f>(O$6*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <v>35756.978861821895</v>
+      </c>
+      <c r="P52">
+        <f>(P$6*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <v>35048.326439999997</v>
+      </c>
+      <c r="Q52">
+        <f>(Q$6*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <v>32041.47257772553</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B53" s="7">
+        <f>B52/$B52</f>
+        <v>1</v>
+      </c>
+      <c r="C53" s="7">
+        <f t="shared" ref="C53:Q53" si="66">C52/$B52</f>
+        <v>0.99117433142557099</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" si="66"/>
+        <v>1.0112328274422622</v>
+      </c>
+      <c r="E53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.97612098184230256</v>
+      </c>
+      <c r="F53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.92797896062899166</v>
+      </c>
+      <c r="G53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.8993022313141279</v>
+      </c>
+      <c r="H53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.88141899510200894</v>
+      </c>
+      <c r="I53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.86110504169926727</v>
+      </c>
+      <c r="J53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.85277713994202098</v>
+      </c>
+      <c r="K53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.84624542998719976</v>
+      </c>
+      <c r="L53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.8592497061727411</v>
+      </c>
+      <c r="M53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.84813020185023802</v>
+      </c>
+      <c r="N53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.84352939772612412</v>
+      </c>
+      <c r="O53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.84778383625724674</v>
+      </c>
+      <c r="P53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.83098196742300301</v>
+      </c>
+      <c r="Q53" s="7">
+        <f t="shared" si="66"/>
+        <v>0.75969065077472386</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54">
+        <f>(B$8*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <v>48507</v>
+      </c>
+      <c r="C54">
+        <f>(C$8*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <v>47936.393854748603</v>
+      </c>
+      <c r="D54">
+        <f>(D$8*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <v>48905.323350491344</v>
+      </c>
+      <c r="E54">
+        <f>(E$8*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <v>47207.083631484791</v>
+      </c>
+      <c r="F54">
+        <f>(F$8*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <v>44878.843112244896</v>
+      </c>
+      <c r="G54">
+        <f>(G$8*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <v>43491.981458590853</v>
+      </c>
+      <c r="H54">
+        <f>(H$8*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <v>42627.668132746898</v>
+      </c>
+      <c r="I54">
+        <f>(I$8*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <v>41645.233593749996</v>
+      </c>
+      <c r="J54">
+        <f>(J$8*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <v>41242.475048355896</v>
+      </c>
+      <c r="K54">
+        <f>(K$8*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <v>40926.588369441277</v>
+      </c>
+      <c r="L54">
+        <f>(L$8*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <v>45928.649324036691</v>
+      </c>
+      <c r="M54">
+        <f>(M$8*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <v>45333.184457386349</v>
+      </c>
+      <c r="N54">
+        <f>(N$8*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <v>45087.391776315788</v>
+      </c>
+      <c r="O54">
+        <f>(O$8*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <v>45313.981895598765</v>
+      </c>
+      <c r="P54">
+        <f>(P$8*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <v>44417.162276065566</v>
+      </c>
+      <c r="Q54">
+        <f>(Q$8*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <v>40605.604155744928</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" s="7">
+        <f>B54/$B54</f>
+        <v>1</v>
+      </c>
+      <c r="C55" s="7">
+        <f t="shared" ref="C55:Q55" si="67">C54/$B54</f>
+        <v>0.98823662264721801</v>
+      </c>
+      <c r="D55" s="7">
+        <f t="shared" si="67"/>
+        <v>1.0082116673983414</v>
+      </c>
+      <c r="E55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.97320146847846267</v>
+      </c>
+      <c r="F55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.92520343686983109</v>
+      </c>
+      <c r="G55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.89661247775766084</v>
+      </c>
+      <c r="H55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.8787941561578102</v>
+      </c>
+      <c r="I55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.8585406970901106</v>
+      </c>
+      <c r="J55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.85023759557086398</v>
+      </c>
+      <c r="K55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.84372540807391261</v>
+      </c>
+      <c r="L55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.94684580213240754</v>
+      </c>
+      <c r="M55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.93456994778869751</v>
+      </c>
+      <c r="N55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.92950278879988013</v>
+      </c>
+      <c r="O55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.93417407581583611</v>
+      </c>
+      <c r="P55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.91568561807709337</v>
+      </c>
+      <c r="Q55" s="7">
+        <f t="shared" si="67"/>
+        <v>0.83710813193446154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <f>(B$11*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <v>56119.5</v>
+      </c>
+      <c r="C56">
+        <f>(C$11*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <v>55308.782122905024</v>
+      </c>
+      <c r="D56">
+        <f>(D$11*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <v>56427.322882545624</v>
+      </c>
+      <c r="E56">
+        <f>(E$11*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <v>54468.112701252234</v>
+      </c>
+      <c r="F56">
+        <f>(F$11*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <v>51781.760204081635</v>
+      </c>
+      <c r="G56">
+        <f>(G$11*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <v>50181.58220024722</v>
+      </c>
+      <c r="H56">
+        <f>(H$11*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <v>49183.769292283083</v>
+      </c>
+      <c r="I56">
+        <f>(I$11*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <v>48050.237109374997</v>
+      </c>
+      <c r="J56">
+        <f>(J$11*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <v>47585.534622823987</v>
+      </c>
+      <c r="K56">
+        <f>(K$11*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <v>47221.174458380839</v>
+      </c>
+      <c r="L56">
+        <f>(L$11*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <v>45928.649324036691</v>
+      </c>
+      <c r="M56">
+        <f>(M$11*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <v>45333.184457386349</v>
+      </c>
+      <c r="N56">
+        <f>(N$11*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <v>45087.391776315788</v>
+      </c>
+      <c r="O56">
+        <f>(O$11*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <v>45313.981895598765</v>
+      </c>
+      <c r="P56">
+        <f>(P$11*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <v>47134.568689180327</v>
+      </c>
+      <c r="Q56">
+        <f>(Q$11*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <v>46480.311885982948</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57" s="7">
+        <f>B56/$B56</f>
+        <v>1</v>
+      </c>
+      <c r="C57" s="7">
+        <f t="shared" ref="C57:Q57" si="68">C56/$B56</f>
+        <v>0.98555372237644712</v>
+      </c>
+      <c r="D57" s="7">
+        <f t="shared" si="68"/>
+        <v>1.0054851323077652</v>
+      </c>
+      <c r="E57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.97057373464218732</v>
+      </c>
+      <c r="F57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.92270530215133129</v>
+      </c>
+      <c r="G57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.894191541269028</v>
+      </c>
+      <c r="H57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.87641139518853661</v>
+      </c>
+      <c r="I57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.85621285131505087</v>
+      </c>
+      <c r="J57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.84793226281103695</v>
+      </c>
+      <c r="K57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.84143968599828656</v>
+      </c>
+      <c r="L57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.81840802794103107</v>
+      </c>
+      <c r="M57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.80779736913882605</v>
+      </c>
+      <c r="N57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.80341756031888711</v>
+      </c>
+      <c r="O57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.80745519642189911</v>
+      </c>
+      <c r="P57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.83989644756600335</v>
+      </c>
+      <c r="Q57" s="7">
+        <f t="shared" si="68"/>
+        <v>0.82823816830126695</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59">
         <f>(B$4*(1+B$21+B$26+B$27+B$28))*B$33</f>
         <v>31578</v>
       </c>
-      <c r="C36">
-        <f>(C$4*(1+C$21+C$26+C$27+C$28))*C$33</f>
-        <v>31670.217237308145</v>
-      </c>
-      <c r="D36">
-        <f>(D$4*(1+D$21+D$26+D$27+D$28))*D$33</f>
-        <v>31440.103926096999</v>
-      </c>
-      <c r="E36">
-        <f>(E$4*(1+E$21+E$26+E$27+E$28))*E$33</f>
-        <v>30760.093959731541</v>
-      </c>
-      <c r="F36">
-        <f>(F$4*(1+F$21+F$26+F$27+F$28))*F$33</f>
-        <v>29442.745182012848</v>
-      </c>
-      <c r="G36">
-        <f>(G$4*(1+G$21+G$26+G$27+G$28))*G$33</f>
-        <v>28615.529656607701</v>
-      </c>
-      <c r="H36">
-        <f>(H$4*(1+H$21+H$26+H$27+H$28))*H$33</f>
-        <v>28197.331979695431</v>
-      </c>
-      <c r="I36">
-        <f>(I$4*(1+I$21+I$26+I$27+I$28))*I$33</f>
-        <v>27774.371999999999</v>
-      </c>
-      <c r="J36">
-        <f>(J$4*(1+J$21+J$26+J$27+J$28))*J$33</f>
-        <v>27774.371999999999</v>
-      </c>
-      <c r="K36">
-        <f>(K$4*(1+K$21+K$26+K$27+K$28))*K$33</f>
-        <v>27856.677259185697</v>
-      </c>
-      <c r="L36">
-        <f>(L$4*(1+L$21+L$26+L$27+L$28))*L$33</f>
-        <v>27602.321442940032</v>
-      </c>
-      <c r="M36">
-        <f>(M$4*(1+M$21+M$26+M$27+M$28))*M$33</f>
-        <v>27489.439195467414</v>
-      </c>
-      <c r="N36">
-        <f>(N$4*(1+N$21+N$26+N$27+N$28))*N$33</f>
-        <v>27545.109667903522</v>
-      </c>
-      <c r="O36">
-        <f>(O$4*(1+O$21+O$26+O$27+O$28))*O$33</f>
-        <v>27863.603232750684</v>
-      </c>
-      <c r="P36">
-        <f>(P$4*(1+P$21+P$26+P$27+P$28))*P$33</f>
-        <v>27682.474537634407</v>
-      </c>
-      <c r="Q36">
-        <f>(Q$4*(1+Q$21+Q$26+Q$27+Q$28))*Q$33</f>
-        <v>25892.63996055875</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="C59">
+        <f t="shared" ref="C59:Q59" si="69">(C$4*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <v>32793</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="69"/>
+        <v>33285</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="69"/>
+        <v>29662.941176470584</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="69"/>
+        <v>25213.499999999996</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="69"/>
+        <v>25213.499999999996</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="69"/>
+        <v>25465.499999999996</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="69"/>
+        <v>20372.399999999998</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="69"/>
+        <v>20372.399999999998</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="69"/>
+        <v>20575.8</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="69"/>
+        <v>17445.476999999999</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="69"/>
+        <v>21353.043599999997</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="69"/>
+        <v>21780.167399999995</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="69"/>
+        <v>22215.943799999997</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="69"/>
+        <v>22660.372800000001</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="69"/>
+        <v>23113.454399999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="7">
-        <f>B36/$B36</f>
+      <c r="B60" s="7">
+        <f t="shared" ref="B60" si="70">B59/$B59</f>
         <v>1</v>
       </c>
-      <c r="C37" s="7">
-        <f t="shared" ref="C37" si="0">C36/$B36</f>
-        <v>1.0029203001237617</v>
-      </c>
-      <c r="D37" s="7">
-        <f t="shared" ref="D37" si="1">D36/$B36</f>
-        <v>0.99563315998787127</v>
-      </c>
-      <c r="E37" s="7">
-        <f t="shared" ref="E37" si="2">E36/$B36</f>
-        <v>0.97409886502411613</v>
-      </c>
-      <c r="F37" s="7">
-        <f t="shared" ref="F37" si="3">F36/$B36</f>
-        <v>0.93238156887747314</v>
-      </c>
-      <c r="G37" s="7">
-        <f t="shared" ref="G37" si="4">G36/$B36</f>
-        <v>0.90618562469465136</v>
-      </c>
-      <c r="H37" s="7">
-        <f t="shared" ref="H37" si="5">H36/$B36</f>
-        <v>0.89294230095938409</v>
-      </c>
-      <c r="I37" s="7">
-        <f t="shared" ref="I37" si="6">I36/$B36</f>
-        <v>0.87954816644499334</v>
-      </c>
-      <c r="J37" s="7">
-        <f t="shared" ref="J37" si="7">J36/$B36</f>
-        <v>0.87954816644499334</v>
-      </c>
-      <c r="K37" s="7">
-        <f t="shared" ref="K37" si="8">K36/$B36</f>
-        <v>0.88215457784488238</v>
-      </c>
-      <c r="L37" s="7">
-        <f t="shared" ref="L37" si="9">L36/$B36</f>
-        <v>0.87409973535182828</v>
-      </c>
-      <c r="M37" s="7">
-        <f t="shared" ref="M37" si="10">M36/$B36</f>
-        <v>0.87052502360717632</v>
-      </c>
-      <c r="N37" s="7">
-        <f t="shared" ref="N37" si="11">N36/$B36</f>
-        <v>0.87228797478952191</v>
-      </c>
-      <c r="O37" s="7">
-        <f t="shared" ref="O37" si="12">O36/$B36</f>
-        <v>0.88237390692097928</v>
-      </c>
-      <c r="P37" s="7">
-        <f t="shared" ref="P37" si="13">P36/$B36</f>
-        <v>0.8766379928315412</v>
-      </c>
-      <c r="Q37" s="7">
-        <f t="shared" ref="Q37" si="14">Q36/$B36</f>
-        <v>0.81995819749695198</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38">
+      <c r="C60" s="7">
+        <f t="shared" ref="C60" si="71">C59/$B59</f>
+        <v>1.0384761542846286</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" ref="D60" si="72">D59/$B59</f>
+        <v>1.0540566216986509</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" ref="E60" si="73">E59/$B59</f>
+        <v>0.93935465122777195</v>
+      </c>
+      <c r="F60" s="7">
+        <f t="shared" ref="F60" si="74">F59/$B59</f>
+        <v>0.79845145354360614</v>
+      </c>
+      <c r="G60" s="7">
+        <f t="shared" ref="G60" si="75">G59/$B59</f>
+        <v>0.79845145354360614</v>
+      </c>
+      <c r="H60" s="7">
+        <f t="shared" ref="H60" si="76">H59/$B59</f>
+        <v>0.80643169295078843</v>
+      </c>
+      <c r="I60" s="7">
+        <f t="shared" ref="I60" si="77">I59/$B59</f>
+        <v>0.6451453543606307</v>
+      </c>
+      <c r="J60" s="7">
+        <f t="shared" ref="J60" si="78">J59/$B59</f>
+        <v>0.6451453543606307</v>
+      </c>
+      <c r="K60" s="7">
+        <f t="shared" ref="K60" si="79">K59/$B59</f>
+        <v>0.65158654759642787</v>
+      </c>
+      <c r="L60" s="7">
+        <f t="shared" ref="L60" si="80">L59/$B59</f>
+        <v>0.55245667870036097</v>
+      </c>
+      <c r="M60" s="7">
+        <f t="shared" ref="M60" si="81">M59/$B59</f>
+        <v>0.67619999999999991</v>
+      </c>
+      <c r="N60" s="7">
+        <f t="shared" ref="N60" si="82">N59/$B59</f>
+        <v>0.68972599277978319</v>
+      </c>
+      <c r="O60" s="7">
+        <f t="shared" ref="O60" si="83">O59/$B59</f>
+        <v>0.70352599277978334</v>
+      </c>
+      <c r="P60" s="7">
+        <f t="shared" ref="P60" si="84">P59/$B59</f>
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="Q60" s="7">
+        <f t="shared" ref="Q60" si="85">Q59/$B59</f>
+        <v>0.73194801444043323</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61">
         <f>(B$5*(1+B$21+B$26+B$27+B$28))*B$33</f>
         <v>39405</v>
       </c>
-      <c r="C38">
-        <f>(C$5*(1+C$21+C$26+C$27+C$28))*C$33</f>
-        <v>39281.383707201887</v>
-      </c>
-      <c r="D38">
-        <f>(D$5*(1+D$21+D$26+D$27+D$28))*D$33</f>
-        <v>38996.213625866054</v>
-      </c>
-      <c r="E38">
-        <f>(E$5*(1+E$21+E$26+E$27+E$28))*E$33</f>
-        <v>38152.288590604025</v>
-      </c>
-      <c r="F38">
-        <f>(F$5*(1+F$21+F$26+F$27+F$28))*F$33</f>
-        <v>36518.357601713062</v>
-      </c>
-      <c r="G38">
-        <f>(G$5*(1+G$21+G$26+G$27+G$28))*G$33</f>
-        <v>35492.347554630593</v>
-      </c>
-      <c r="H38">
-        <f>(H$5*(1+H$21+H$26+H$27+H$28))*H$33</f>
-        <v>34973.85989847716</v>
-      </c>
-      <c r="I38">
-        <f>(I$5*(1+I$21+I$26+I$27+I$28))*I$33</f>
-        <v>34449.252</v>
-      </c>
-      <c r="J38">
-        <f>(J$5*(1+J$21+J$26+J$27+J$28))*J$33</f>
-        <v>34449.252</v>
-      </c>
-      <c r="K38">
-        <f>(K$5*(1+K$21+K$26+K$27+K$28))*K$33</f>
-        <v>34552.173783515391</v>
-      </c>
-      <c r="L38">
-        <f>(L$5*(1+L$21+L$26+L$27+L$28))*L$33</f>
-        <v>31948.95588974854</v>
-      </c>
-      <c r="M38">
-        <f>(M$5*(1+M$21+M$26+M$27+M$28))*M$33</f>
-        <v>31819.537257790362</v>
-      </c>
-      <c r="N38">
-        <f>(N$5*(1+N$21+N$26+N$27+N$28))*N$33</f>
-        <v>31883.447031539887</v>
-      </c>
-      <c r="O38">
-        <f>(O$5*(1+O$21+O$26+O$27+O$28))*O$33</f>
-        <v>32251.851902483897</v>
-      </c>
-      <c r="P38">
-        <f>(P$5*(1+P$21+P$26+P$27+P$28))*P$33</f>
-        <v>32042.214435483867</v>
-      </c>
-      <c r="Q38">
-        <f>(Q$5*(1+Q$21+Q$26+Q$27+Q$28))*Q$33</f>
-        <v>29970.748377978634</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="C61">
+        <f t="shared" ref="C61:Q61" si="86">(C$5*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <v>40674</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="86"/>
+        <v>41284.5</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="86"/>
+        <v>36791.470588235286</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="86"/>
+        <v>31272.749999999996</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="86"/>
+        <v>31272.749999999996</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="86"/>
+        <v>31585.499999999996</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="86"/>
+        <v>25268.399999999998</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="86"/>
+        <v>25268.399999999998</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="86"/>
+        <v>25521.3</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="86"/>
+        <v>20192.677499999998</v>
+      </c>
+      <c r="M61">
+        <f t="shared" si="86"/>
+        <v>24716.545199999997</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="86"/>
+        <v>25210.529999999995</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="86"/>
+        <v>25714.740599999997</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="86"/>
+        <v>26229.177</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="86"/>
+        <v>26753.839199999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="7">
-        <f>B38/$B38</f>
+      <c r="B62" s="7">
+        <f t="shared" ref="B62" si="87">B61/$B61</f>
         <v>1</v>
       </c>
-      <c r="C39" s="7">
-        <f t="shared" ref="C39" si="15">C38/$B38</f>
-        <v>0.99686292874513105</v>
-      </c>
-      <c r="D39" s="7">
-        <f t="shared" ref="D39" si="16">D38/$B38</f>
-        <v>0.98962602781033004</v>
-      </c>
-      <c r="E39" s="7">
-        <f t="shared" ref="E39" si="17">E38/$B38</f>
-        <v>0.96820932852693886</v>
-      </c>
-      <c r="F39" s="7">
-        <f t="shared" ref="F39" si="18">F38/$B38</f>
-        <v>0.92674426092407214</v>
-      </c>
-      <c r="G39" s="7">
-        <f t="shared" ref="G39" si="19">G38/$B38</f>
-        <v>0.90070670104379125</v>
-      </c>
-      <c r="H39" s="7">
-        <f t="shared" ref="H39" si="20">H38/$B38</f>
-        <v>0.88754878564844963</v>
-      </c>
-      <c r="I39" s="7">
-        <f t="shared" ref="I39" si="21">I38/$B38</f>
-        <v>0.87423555386372287</v>
-      </c>
-      <c r="J39" s="7">
-        <f t="shared" ref="J39" si="22">J38/$B38</f>
-        <v>0.87423555386372287</v>
-      </c>
-      <c r="K39" s="7">
-        <f t="shared" ref="K39" si="23">K38/$B38</f>
-        <v>0.87684745041277479</v>
-      </c>
-      <c r="L39" s="7">
-        <f t="shared" ref="L39" si="24">L38/$B38</f>
-        <v>0.81078431391317196</v>
-      </c>
-      <c r="M39" s="7">
-        <f t="shared" ref="M39" si="25">M38/$B38</f>
-        <v>0.80749999385332727</v>
-      </c>
-      <c r="N39" s="7">
-        <f t="shared" ref="N39" si="26">N38/$B38</f>
-        <v>0.80912186350818138</v>
-      </c>
-      <c r="O39" s="7">
-        <f t="shared" ref="O39" si="27">O38/$B38</f>
-        <v>0.81847105449775148</v>
-      </c>
-      <c r="P39" s="7">
-        <f t="shared" ref="P39" si="28">P38/$B38</f>
-        <v>0.81315098174048639</v>
-      </c>
-      <c r="Q39" s="7">
-        <f t="shared" ref="Q39" si="29">Q38/$B38</f>
-        <v>0.76058237223648351</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40">
+      <c r="C62" s="7">
+        <f t="shared" ref="C62" si="88">C61/$B61</f>
+        <v>1.0322040350209365</v>
+      </c>
+      <c r="D62" s="7">
+        <f t="shared" ref="D62" si="89">D61/$B61</f>
+        <v>1.0476969927674153</v>
+      </c>
+      <c r="E62" s="7">
+        <f t="shared" ref="E62" si="90">E61/$B61</f>
+        <v>0.93367518305380759</v>
+      </c>
+      <c r="F62" s="7">
+        <f t="shared" ref="F62" si="91">F61/$B61</f>
+        <v>0.79362390559573648</v>
+      </c>
+      <c r="G62" s="7">
+        <f t="shared" ref="G62" si="92">G61/$B61</f>
+        <v>0.79362390559573648</v>
+      </c>
+      <c r="H62" s="7">
+        <f t="shared" ref="H62" si="93">H61/$B61</f>
+        <v>0.80156071564522258</v>
+      </c>
+      <c r="I62" s="7">
+        <f t="shared" ref="I62" si="94">I61/$B61</f>
+        <v>0.64124857251617806</v>
+      </c>
+      <c r="J62" s="7">
+        <f t="shared" ref="J62" si="95">J61/$B61</f>
+        <v>0.64124857251617806</v>
+      </c>
+      <c r="K62" s="7">
+        <f t="shared" ref="K62" si="96">K61/$B61</f>
+        <v>0.64766653977921584</v>
+      </c>
+      <c r="L62" s="7">
+        <f t="shared" ref="L62" si="97">L61/$B61</f>
+        <v>0.51243947468595352</v>
+      </c>
+      <c r="M62" s="7">
+        <f t="shared" ref="M62" si="98">M61/$B61</f>
+        <v>0.6272438827559953</v>
+      </c>
+      <c r="N62" s="7">
+        <f t="shared" ref="N62" si="99">N61/$B61</f>
+        <v>0.63977997716025869</v>
+      </c>
+      <c r="O62" s="7">
+        <f t="shared" ref="O62" si="100">O61/$B61</f>
+        <v>0.652575576703464</v>
+      </c>
+      <c r="P62" s="7">
+        <f t="shared" ref="P62" si="101">P61/$B61</f>
+        <v>0.66563068138561099</v>
+      </c>
+      <c r="Q62" s="7">
+        <f t="shared" ref="Q62" si="102">Q61/$B61</f>
+        <v>0.67894529120669966</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63">
         <f>(B$6*(1+B$21+B$26+B$27+B$28))*B$33</f>
         <v>42177</v>
       </c>
-      <c r="C40">
-        <f>(C$6*(1+C$21+C$26+C$27+C$28))*C$33</f>
-        <v>41975.858323494685</v>
-      </c>
-      <c r="D40">
-        <f>(D$6*(1+D$21+D$26+D$27+D$28))*D$33</f>
-        <v>41671.243648960743</v>
-      </c>
-      <c r="E40">
-        <f>(E$6*(1+E$21+E$26+E$27+E$28))*E$33</f>
-        <v>40769.614093959732</v>
-      </c>
-      <c r="F40">
-        <f>(F$6*(1+F$21+F$26+F$27+F$28))*F$33</f>
-        <v>39023.592077087793</v>
-      </c>
-      <c r="G40">
-        <f>(G$6*(1+G$21+G$26+G$27+G$28))*G$33</f>
-        <v>37927.195629552552</v>
-      </c>
-      <c r="H40">
-        <f>(H$6*(1+H$21+H$26+H$27+H$28))*H$33</f>
-        <v>37373.049746192897</v>
-      </c>
-      <c r="I40">
-        <f>(I$6*(1+I$21+I$26+I$27+I$28))*I$33</f>
-        <v>36812.453999999998</v>
-      </c>
-      <c r="J40">
-        <f>(J$6*(1+J$21+J$26+J$27+J$28))*J$33</f>
-        <v>36812.453999999998</v>
-      </c>
-      <c r="K40">
-        <f>(K$6*(1+K$21+K$26+K$27+K$28))*K$33</f>
-        <v>36922.099304865937</v>
-      </c>
-      <c r="L40">
-        <f>(L$6*(1+L$21+L$26+L$27+L$28))*L$33</f>
-        <v>37814.993692456475</v>
-      </c>
-      <c r="M40">
-        <f>(M$6*(1+M$21+M$26+M$27+M$28))*M$33</f>
-        <v>37661.524096317276</v>
-      </c>
-      <c r="N40">
-        <f>(N$6*(1+N$21+N$26+N$27+N$28))*N$33</f>
-        <v>37737.864684601111</v>
-      </c>
-      <c r="O40">
-        <f>(O$6*(1+O$21+O$26+O$27+O$28))*O$33</f>
-        <v>38174.211786568529</v>
-      </c>
-      <c r="P40">
-        <f>(P$6*(1+P$21+P$26+P$27+P$28))*P$33</f>
-        <v>37925.028553763441</v>
-      </c>
-      <c r="Q40">
-        <f>(Q$6*(1+Q$21+Q$26+Q$27+Q$28))*Q$33</f>
-        <v>35473.727433032043</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="C63">
+        <f t="shared" ref="C63:Q63" si="103">(C$6*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <v>43464</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="103"/>
+        <v>44116.5</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="103"/>
+        <v>39315.44117647058</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="103"/>
+        <v>33418.124999999993</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="103"/>
+        <v>33418.124999999993</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="103"/>
+        <v>33752.249999999993</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="103"/>
+        <v>27001.8</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="103"/>
+        <v>27001.8</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="103"/>
+        <v>27271.8</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="103"/>
+        <v>23900.1855</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="103"/>
+        <v>29254.440599999998</v>
+      </c>
+      <c r="N63">
+        <f t="shared" si="103"/>
+        <v>29839.670999999995</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="103"/>
+        <v>30436.700399999994</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="103"/>
+        <v>31044.742200000001</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="103"/>
+        <v>31666.156199999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="7">
-        <f>B40/$B40</f>
+      <c r="B64" s="7">
+        <f>B63/$B63</f>
         <v>1</v>
       </c>
-      <c r="C41" s="7">
-        <f t="shared" ref="C41:Q41" si="30">C40/$B40</f>
-        <v>0.99523101034911643</v>
-      </c>
-      <c r="D41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.98800871681155</v>
-      </c>
-      <c r="E41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.9666314364217401</v>
-      </c>
-      <c r="F41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.92523394449789675</v>
-      </c>
-      <c r="G41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.89923881806559391</v>
-      </c>
-      <c r="H41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.88610023819126293</v>
-      </c>
-      <c r="I41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.87280873461839381</v>
-      </c>
-      <c r="J41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.87280873461839381</v>
-      </c>
-      <c r="K41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.87540838146065236</v>
-      </c>
-      <c r="L41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.89657855448363977</v>
-      </c>
-      <c r="M41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.89293985101636619</v>
-      </c>
-      <c r="N41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.89474985619178959</v>
-      </c>
-      <c r="O41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.90509547351799624</v>
-      </c>
-      <c r="P41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.89918743755514718</v>
-      </c>
-      <c r="Q41" s="7">
-        <f t="shared" si="30"/>
-        <v>0.84106805683268238</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42">
+      <c r="C64" s="7">
+        <f t="shared" ref="C64:Q64" si="104">C63/$B63</f>
+        <v>1.0305142613272638</v>
+      </c>
+      <c r="D64" s="7">
+        <f t="shared" si="104"/>
+        <v>1.0459847784337435</v>
+      </c>
+      <c r="E64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.93215357129408394</v>
+      </c>
+      <c r="F64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.79233053559997135</v>
+      </c>
+      <c r="G64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.79233053559997135</v>
+      </c>
+      <c r="H64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.8002525072907033</v>
+      </c>
+      <c r="I64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.6402020058325627</v>
+      </c>
+      <c r="J64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.6402020058325627</v>
+      </c>
+      <c r="K64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.64660359911800269</v>
+      </c>
+      <c r="L64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.56666395191692154</v>
+      </c>
+      <c r="M64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.6936112241268938</v>
+      </c>
+      <c r="N64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.70748680560495047</v>
+      </c>
+      <c r="O64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.72164213670958088</v>
+      </c>
+      <c r="P64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.73605856746568032</v>
+      </c>
+      <c r="Q64" s="7">
+        <f t="shared" si="104"/>
+        <v>0.75079204779856312</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65">
         <f>(B$8*(1+B$21+B$26+B$27+B$28))*B$33</f>
         <v>48507</v>
       </c>
-      <c r="C42">
-        <f>(C$8*(1+C$21+C$26+C$27+C$28))*C$33</f>
-        <v>48132.587957497046</v>
-      </c>
-      <c r="D42">
-        <f>(D$8*(1+D$21+D$26+D$27+D$28))*D$33</f>
-        <v>47782.15704387991</v>
-      </c>
-      <c r="E42">
-        <f>(E$8*(1+E$21+E$26+E$27+E$28))*E$33</f>
-        <v>46748.151006711407</v>
-      </c>
-      <c r="F42">
-        <f>(F$8*(1+F$21+F$26+F$27+F$28))*F$33</f>
-        <v>44746.088865096361</v>
-      </c>
-      <c r="G42">
-        <f>(G$8*(1+G$21+G$26+G$27+G$28))*G$33</f>
-        <v>43488.914672216444</v>
-      </c>
-      <c r="H42">
-        <f>(H$8*(1+H$21+H$26+H$27+H$28))*H$33</f>
-        <v>42854.064974619294</v>
-      </c>
-      <c r="I42">
-        <f>(I$8*(1+I$21+I$26+I$27+I$28))*I$33</f>
-        <v>42211.254000000001</v>
-      </c>
-      <c r="J42">
-        <f>(J$8*(1+J$21+J$26+J$27+J$28))*J$33</f>
-        <v>42211.254000000001</v>
-      </c>
-      <c r="K42">
-        <f>(K$8*(1+K$21+K$26+K$27+K$28))*K$33</f>
-        <v>42336.983118172786</v>
-      </c>
-      <c r="L42">
-        <f>(L$8*(1+L$21+L$26+L$27+L$28))*L$33</f>
-        <v>47923.952402321069</v>
-      </c>
-      <c r="M42">
-        <f>(M$8*(1+M$21+M$26+M$27+M$28))*M$33</f>
-        <v>47728.293235127472</v>
-      </c>
-      <c r="N42">
-        <f>(N$8*(1+N$21+N$26+N$27+N$28))*N$33</f>
-        <v>47825.170547309834</v>
-      </c>
-      <c r="O42">
-        <f>(O$8*(1+O$21+O$26+O$27+O$28))*O$33</f>
-        <v>48377.284570377175</v>
-      </c>
-      <c r="P42">
-        <f>(P$8*(1+P$21+P$26+P$27+P$28))*P$33</f>
-        <v>48062.841188172039</v>
-      </c>
-      <c r="Q42">
-        <f>(Q$8*(1+Q$21+Q$26+Q$27+Q$28))*Q$33</f>
-        <v>44955.241385373869</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="C65">
+        <f t="shared" ref="C65:Q65" si="105">(C$8*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <v>49839</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="105"/>
+        <v>50586</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="105"/>
+        <v>45080.735294117643</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="105"/>
+        <v>38318.624999999993</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="105"/>
+        <v>38318.624999999993</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="105"/>
+        <v>38702.249999999993</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="105"/>
+        <v>30961.8</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="105"/>
+        <v>30961.8</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="105"/>
+        <v>31271.399999999998</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="105"/>
+        <v>30289.343999999997</v>
+      </c>
+      <c r="M65">
+        <f t="shared" si="105"/>
+        <v>37074.031199999998</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="105"/>
+        <v>37815.794999999998</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="105"/>
+        <v>38571.717599999996</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="105"/>
+        <v>39343.372199999998</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="105"/>
+        <v>40129.972199999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="7">
-        <f>B42/$B42</f>
+      <c r="B66" s="7">
+        <f>B65/$B65</f>
         <v>1</v>
       </c>
-      <c r="C43" s="7">
-        <f t="shared" ref="C43:Q43" si="31">C42/$B42</f>
-        <v>0.992281278114438</v>
-      </c>
-      <c r="D43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.98505694114003983</v>
-      </c>
-      <c r="E43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.96374030566127378</v>
-      </c>
-      <c r="F43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.92246663090061976</v>
-      </c>
-      <c r="G43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.89654925417396347</v>
-      </c>
-      <c r="H43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.88346145864760328</v>
-      </c>
-      <c r="I43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.87020953676788915</v>
-      </c>
-      <c r="J43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.87020953676788915</v>
-      </c>
-      <c r="K43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.87280151561986485</v>
-      </c>
-      <c r="L43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.98798013487375158</v>
-      </c>
-      <c r="M43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.98394650741392942</v>
-      </c>
-      <c r="N43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.98594368951511813</v>
-      </c>
-      <c r="O43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.997325841020413</v>
-      </c>
-      <c r="P43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.99084340792405301</v>
-      </c>
-      <c r="Q43" s="7">
-        <f t="shared" si="31"/>
-        <v>0.9267784316773634</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44">
+      <c r="C66" s="7">
+        <f t="shared" ref="C66:Q66" si="106">C65/$B65</f>
+        <v>1.0274599542334095</v>
+      </c>
+      <c r="D66" s="7">
+        <f t="shared" si="106"/>
+        <v>1.0428597934318757</v>
+      </c>
+      <c r="E66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.92936556155024308</v>
+      </c>
+      <c r="F66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.78996072731770661</v>
+      </c>
+      <c r="G66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.78996072731770661</v>
+      </c>
+      <c r="H66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.79786937967715987</v>
+      </c>
+      <c r="I66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.63829550374172794</v>
+      </c>
+      <c r="J66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.63829550374172794</v>
+      </c>
+      <c r="K66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.64467808769868262</v>
+      </c>
+      <c r="L66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.6244324324324324</v>
+      </c>
+      <c r="M66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.76430270270270262</v>
+      </c>
+      <c r="N66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.77959459459459457</v>
+      </c>
+      <c r="O66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.79517837837837835</v>
+      </c>
+      <c r="P66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.8110864864864864</v>
+      </c>
+      <c r="Q66" s="7">
+        <f t="shared" si="106"/>
+        <v>0.82730270270270267</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67">
         <f>(B$11*(1+B$21+B$26+B$27+B$28))*B$33</f>
         <v>56119.5</v>
       </c>
-      <c r="C44">
-        <f>(C$11*(1+C$21+C$26+C$27+C$28))*C$33</f>
-        <v>55535.14994096812</v>
-      </c>
-      <c r="D44">
-        <f>(D$11*(1+D$21+D$26+D$27+D$28))*D$33</f>
-        <v>55131.40531177829</v>
-      </c>
-      <c r="E44">
-        <f>(E$11*(1+E$21+E$26+E$27+E$28))*E$33</f>
-        <v>53938.590604026846</v>
-      </c>
-      <c r="F44">
-        <f>(F$11*(1+F$21+F$26+F$27+F$28))*F$33</f>
-        <v>51628.586723768734</v>
-      </c>
-      <c r="G44">
-        <f>(G$11*(1+G$21+G$26+G$27+G$28))*G$33</f>
-        <v>50178.043704474505</v>
-      </c>
-      <c r="H44">
-        <f>(H$11*(1+H$21+H$26+H$27+H$28))*H$33</f>
-        <v>49444.985786802034</v>
-      </c>
-      <c r="I44">
-        <f>(I$11*(1+I$21+I$26+I$27+I$28))*I$33</f>
-        <v>48703.310999999994</v>
-      </c>
-      <c r="J44">
-        <f>(J$11*(1+J$21+J$26+J$27+J$28))*J$33</f>
-        <v>48703.310999999994</v>
-      </c>
-      <c r="K44">
-        <f>(K$11*(1+K$21+K$26+K$27+K$28))*K$33</f>
-        <v>48848.490566037734</v>
-      </c>
-      <c r="L44">
-        <f>(L$11*(1+L$21+L$26+L$27+L$28))*L$33</f>
-        <v>47923.952402321069</v>
-      </c>
-      <c r="M44">
-        <f>(M$11*(1+M$21+M$26+M$27+M$28))*M$33</f>
-        <v>47728.293235127472</v>
-      </c>
-      <c r="N44">
-        <f>(N$11*(1+N$21+N$26+N$27+N$28))*N$33</f>
-        <v>47825.170547309834</v>
-      </c>
-      <c r="O44">
-        <f>(O$11*(1+O$21+O$26+O$27+O$28))*O$33</f>
-        <v>48377.284570377175</v>
-      </c>
-      <c r="P44">
-        <f>(P$11*(1+P$21+P$26+P$27+P$28))*P$33</f>
-        <v>51003.287317204296</v>
-      </c>
-      <c r="Q44">
-        <f>(Q$11*(1+Q$21+Q$26+Q$27+Q$28))*Q$33</f>
-        <v>51459.242731306484</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="C67">
+        <f t="shared" ref="C67:Q67" si="107">(C$11*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <v>57504</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="107"/>
+        <v>58366.5</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="107"/>
+        <v>52014.70588235293</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="107"/>
+        <v>44212.499999999993</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="107"/>
+        <v>44212.499999999993</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="107"/>
+        <v>44654.624999999993</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="107"/>
+        <v>35723.699999999997</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="107"/>
+        <v>35723.699999999997</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="107"/>
+        <v>36081</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="107"/>
+        <v>30289.343999999997</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="107"/>
+        <v>37074.031199999998</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="107"/>
+        <v>37815.794999999998</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="107"/>
+        <v>38571.717599999996</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="107"/>
+        <v>41750.368199999997</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="107"/>
+        <v>45935.866799999996</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="7">
-        <f>B44/$B44</f>
+      <c r="B68" s="7">
+        <f>B67/$B67</f>
         <v>1</v>
       </c>
-      <c r="C45" s="7">
-        <f t="shared" ref="C45:Q45" si="32">C44/$B44</f>
-        <v>0.98958739726776113</v>
-      </c>
-      <c r="D45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.98239302402513007</v>
-      </c>
-      <c r="E45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.9611381178383066</v>
-      </c>
-      <c r="F45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.91997588581097001</v>
-      </c>
-      <c r="G45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.89412848839484504</v>
-      </c>
-      <c r="H45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.88106604276235589</v>
-      </c>
-      <c r="I45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.86785005212092048</v>
-      </c>
-      <c r="J45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.86785005212092048</v>
-      </c>
-      <c r="K45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.87043702395847666</v>
-      </c>
-      <c r="L45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.85396256920181168</v>
-      </c>
-      <c r="M45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.85047609538801083</v>
-      </c>
-      <c r="N45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.85220236365808377</v>
-      </c>
-      <c r="O45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.86204054865736823</v>
-      </c>
-      <c r="P45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.90883360181762662</v>
-      </c>
-      <c r="Q45" s="7">
-        <f t="shared" si="32"/>
-        <v>0.91695832520436715</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47">
-        <f>(B$4*(1+B$21+B$26+B$27+B$28))*B$34</f>
-        <v>31578</v>
-      </c>
-      <c r="C47">
-        <f>(C$4*(1+C$21+C$26+C$27+C$28))*C$34</f>
-        <v>31541.12569832402</v>
-      </c>
-      <c r="D47">
-        <f>(D$4*(1+D$21+D$26+D$27+D$28))*D$34</f>
-        <v>32179.134300421152</v>
-      </c>
-      <c r="E47">
-        <f>(E$4*(1+E$21+E$26+E$27+E$28))*E$34</f>
-        <v>31062.069767441859</v>
-      </c>
-      <c r="F47">
-        <f>(F$4*(1+F$21+F$26+F$27+F$28))*F$34</f>
-        <v>29530.09693877551</v>
-      </c>
-      <c r="G47">
-        <f>(G$4*(1+G$21+G$26+G$27+G$28))*G$34</f>
-        <v>28617.547589616814</v>
-      </c>
-      <c r="H47">
-        <f>(H$4*(1+H$21+H$26+H$27+H$28))*H$34</f>
-        <v>28048.3662534986</v>
-      </c>
-      <c r="I47">
-        <f>(I$4*(1+I$21+I$26+I$27+I$28))*I$34</f>
-        <v>27401.939062499998</v>
-      </c>
-      <c r="J47">
-        <f>(J$4*(1+J$21+J$26+J$27+J$28))*J$34</f>
-        <v>27136.929980657638</v>
-      </c>
-      <c r="K47">
-        <f>(K$4*(1+K$21+K$26+K$27+K$28))*K$34</f>
-        <v>26928.672748004559</v>
-      </c>
-      <c r="L47">
-        <f>(L$4*(1+L$21+L$26+L$27+L$28))*L$34</f>
-        <v>26453.104940917427</v>
-      </c>
-      <c r="M47">
-        <f>(M$4*(1+M$21+M$26+M$27+M$28))*M$34</f>
-        <v>26109.9597997159</v>
-      </c>
-      <c r="N47">
-        <f>(N$4*(1+N$21+N$26+N$27+N$28))*N$34</f>
-        <v>25968.274381578944</v>
-      </c>
-      <c r="O47">
-        <f>(O$4*(1+O$21+O$26+O$27+O$28))*O$34</f>
-        <v>26099.249340839298</v>
-      </c>
-      <c r="P47">
-        <f>(P$4*(1+P$21+P$26+P$27+P$28))*P$34</f>
-        <v>25582.694100983605</v>
-      </c>
-      <c r="Q47">
-        <f>(Q$4*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
-        <v>23387.401699676753</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="7">
-        <f t="shared" ref="B48" si="33">B47/$B47</f>
-        <v>1</v>
-      </c>
-      <c r="C48" s="7">
-        <f t="shared" ref="C48" si="34">C47/$B47</f>
-        <v>0.99883227874862313</v>
-      </c>
-      <c r="D48" s="7">
-        <f t="shared" ref="D48" si="35">D47/$B47</f>
-        <v>1.0190364906080547</v>
-      </c>
-      <c r="E48" s="7">
-        <f t="shared" ref="E48" si="36">E47/$B47</f>
-        <v>0.9836617191539001</v>
-      </c>
-      <c r="F48" s="7">
-        <f t="shared" ref="F48" si="37">F47/$B47</f>
-        <v>0.9351477908282827</v>
-      </c>
-      <c r="G48" s="7">
-        <f t="shared" ref="G48" si="38">G47/$B47</f>
-        <v>0.9062495278237005</v>
-      </c>
-      <c r="H48" s="7">
-        <f t="shared" ref="H48" si="39">H47/$B47</f>
-        <v>0.88822491144146554</v>
-      </c>
-      <c r="I48" s="7">
-        <f t="shared" ref="I48" si="40">I47/$B47</f>
-        <v>0.86775410293558797</v>
-      </c>
-      <c r="J48" s="7">
-        <f t="shared" ref="J48" si="41">J47/$B47</f>
-        <v>0.8593618969110659</v>
-      </c>
-      <c r="K48" s="7">
-        <f t="shared" ref="K48" si="42">K47/$B47</f>
-        <v>0.85276688669341183</v>
-      </c>
-      <c r="L48" s="7">
-        <f t="shared" ref="L48" si="43">L47/$B47</f>
-        <v>0.83770678766601514</v>
-      </c>
-      <c r="M48" s="7">
-        <f t="shared" ref="M48" si="44">M47/$B47</f>
-        <v>0.82684019886363602</v>
-      </c>
-      <c r="N48" s="7">
-        <f t="shared" ref="N48" si="45">N47/$B47</f>
-        <v>0.82235335935078036</v>
-      </c>
-      <c r="O48" s="7">
-        <f t="shared" ref="O48" si="46">O47/$B47</f>
-        <v>0.82650102415730253</v>
-      </c>
-      <c r="P48" s="7">
-        <f t="shared" ref="P48" si="47">P47/$B47</f>
-        <v>0.81014295081967203</v>
-      </c>
-      <c r="Q48" s="7">
-        <f t="shared" ref="Q48" si="48">Q47/$B47</f>
-        <v>0.7406232725212728</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>62</v>
-      </c>
-      <c r="B49">
-        <f>(B$5*(1+B$21+B$26+B$27+B$28))*B$34</f>
-        <v>39405</v>
-      </c>
-      <c r="C49">
-        <f>(C$5*(1+C$21+C$26+C$27+C$28))*C$34</f>
-        <v>39121.26815642458</v>
-      </c>
-      <c r="D49">
-        <f>(D$5*(1+D$21+D$26+D$27+D$28))*D$34</f>
-        <v>39912.857744501642</v>
-      </c>
-      <c r="E49">
-        <f>(E$5*(1+E$21+E$26+E$27+E$28))*E$34</f>
-        <v>38526.834525939179</v>
-      </c>
-      <c r="F49">
-        <f>(F$5*(1+F$21+F$26+F$27+F$28))*F$34</f>
-        <v>36626.701530612248</v>
-      </c>
-      <c r="G49">
-        <f>(G$5*(1+G$21+G$26+G$27+G$28))*G$34</f>
-        <v>35494.850432632884</v>
-      </c>
-      <c r="H49">
-        <f>(H$5*(1+H$21+H$26+H$27+H$28))*H$34</f>
-        <v>34789.093962415034</v>
-      </c>
-      <c r="I49">
-        <f>(I$5*(1+I$21+I$26+I$27+I$28))*I$34</f>
-        <v>33987.314062500001</v>
-      </c>
-      <c r="J49">
-        <f>(J$5*(1+J$21+J$26+J$27+J$28))*J$34</f>
-        <v>33658.616634429396</v>
-      </c>
-      <c r="K49">
-        <f>(K$5*(1+K$21+K$26+K$27+K$28))*K$34</f>
-        <v>33401.118586088938</v>
-      </c>
-      <c r="L49">
-        <f>(L$5*(1+L$21+L$26+L$27+L$28))*L$34</f>
-        <v>30618.768231192655</v>
-      </c>
-      <c r="M49">
-        <f>(M$5*(1+M$21+M$26+M$27+M$28))*M$34</f>
-        <v>30222.764194602267</v>
-      </c>
-      <c r="N49">
-        <f>(N$5*(1+N$21+N$26+N$27+N$28))*N$34</f>
-        <v>30058.261184210522</v>
-      </c>
-      <c r="O49">
-        <f>(O$5*(1+O$21+O$26+O$27+O$28))*O$34</f>
-        <v>30209.629295803476</v>
-      </c>
-      <c r="P49">
-        <f>(P$5*(1+P$21+P$26+P$27+P$28))*P$34</f>
-        <v>29611.737531147537</v>
-      </c>
-      <c r="Q49">
-        <f>(Q$5*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
-        <v>27070.933385836022</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="7">
-        <f t="shared" ref="B50" si="49">B49/$B49</f>
-        <v>1</v>
-      </c>
-      <c r="C50" s="7">
-        <f t="shared" ref="C50" si="50">C49/$B49</f>
-        <v>0.99279959792982053</v>
-      </c>
-      <c r="D50" s="7">
-        <f t="shared" ref="D50" si="51">D49/$B49</f>
-        <v>1.0128881549169304</v>
-      </c>
-      <c r="E50" s="7">
-        <f t="shared" ref="E50" si="52">E49/$B49</f>
-        <v>0.97771436431770531</v>
-      </c>
-      <c r="F50" s="7">
-        <f t="shared" ref="F50" si="53">F49/$B49</f>
-        <v>0.92949375791428113</v>
-      </c>
-      <c r="G50" s="7">
-        <f t="shared" ref="G50" si="54">G49/$B49</f>
-        <v>0.90077021780568156</v>
-      </c>
-      <c r="H50" s="7">
-        <f t="shared" ref="H50" si="55">H49/$B49</f>
-        <v>0.88285988992298015</v>
-      </c>
-      <c r="I50" s="7">
-        <f t="shared" ref="I50" si="56">I49/$B49</f>
-        <v>0.86251272839741155</v>
-      </c>
-      <c r="J50" s="7">
-        <f t="shared" ref="J50" si="57">J49/$B49</f>
-        <v>0.85417121264888707</v>
-      </c>
-      <c r="K50" s="7">
-        <f t="shared" ref="K50" si="58">K49/$B49</f>
-        <v>0.84763655845930563</v>
-      </c>
-      <c r="L50" s="7">
-        <f t="shared" ref="L50" si="59">L49/$B49</f>
-        <v>0.77702748968893931</v>
-      </c>
-      <c r="M50" s="7">
-        <f t="shared" ref="M50" si="60">M49/$B49</f>
-        <v>0.76697790114458231</v>
-      </c>
-      <c r="N50" s="7">
-        <f t="shared" ref="N50" si="61">N49/$B49</f>
-        <v>0.76280322761605179</v>
-      </c>
-      <c r="O50" s="7">
-        <f t="shared" ref="O50" si="62">O49/$B49</f>
-        <v>0.76664457037948164</v>
-      </c>
-      <c r="P50" s="7">
-        <f t="shared" ref="P50" si="63">P49/$B49</f>
-        <v>0.75147157800146014</v>
-      </c>
-      <c r="Q50" s="7">
-        <f t="shared" ref="Q50" si="64">Q49/$B49</f>
-        <v>0.68699234578951962</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51">
-        <f>(B$6*(1+B$21+B$26+B$27+B$28))*B$34</f>
-        <v>42177</v>
-      </c>
-      <c r="C51">
-        <f>(C$6*(1+C$21+C$26+C$27+C$28))*C$34</f>
-        <v>41804.75977653631</v>
-      </c>
-      <c r="D51">
-        <f>(D$6*(1+D$21+D$26+D$27+D$28))*D$34</f>
-        <v>42650.766963032293</v>
-      </c>
-      <c r="E51">
-        <f>(E$6*(1+E$21+E$26+E$27+E$28))*E$34</f>
-        <v>41169.854651162794</v>
-      </c>
-      <c r="F51">
-        <f>(F$6*(1+F$21+F$26+F$27+F$28))*F$34</f>
-        <v>39139.368622448979</v>
-      </c>
-      <c r="G51">
-        <f>(G$6*(1+G$21+G$26+G$27+G$28))*G$34</f>
-        <v>37929.870210135974</v>
-      </c>
-      <c r="H51">
-        <f>(H$6*(1+H$21+H$26+H$27+H$28))*H$34</f>
-        <v>37175.608956417433</v>
-      </c>
-      <c r="I51">
-        <f>(I$6*(1+I$21+I$26+I$27+I$28))*I$34</f>
-        <v>36318.827343749996</v>
-      </c>
-      <c r="J51">
-        <f>(J$6*(1+J$21+J$26+J$27+J$28))*J$34</f>
-        <v>35967.58143133462</v>
-      </c>
-      <c r="K51">
-        <f>(K$6*(1+K$21+K$26+K$27+K$28))*K$34</f>
-        <v>35692.093500570125</v>
-      </c>
-      <c r="L51">
-        <f>(L$6*(1+L$21+L$26+L$27+L$28))*L$34</f>
-        <v>36240.574857247702</v>
-      </c>
-      <c r="M51">
-        <f>(M$6*(1+M$21+M$26+M$27+M$28))*M$34</f>
-        <v>35771.587523437491</v>
-      </c>
-      <c r="N51">
-        <f>(N$6*(1+N$21+N$26+N$27+N$28))*N$34</f>
-        <v>35577.539407894736</v>
-      </c>
-      <c r="O51">
-        <f>(O$6*(1+O$21+O$26+O$27+O$28))*O$34</f>
-        <v>35756.978861821895</v>
-      </c>
-      <c r="P51">
-        <f>(P$6*(1+P$21+P$26+P$27+P$28))*P$34</f>
-        <v>35048.326439999997</v>
-      </c>
-      <c r="Q51">
-        <f>(Q$6*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
-        <v>32041.47257772553</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>43</v>
-      </c>
-      <c r="B52" s="7">
-        <f>B51/$B51</f>
-        <v>1</v>
-      </c>
-      <c r="C52" s="7">
-        <f t="shared" ref="C52:Q52" si="65">C51/$B51</f>
-        <v>0.99117433142557099</v>
-      </c>
-      <c r="D52" s="7">
-        <f t="shared" si="65"/>
-        <v>1.0112328274422622</v>
-      </c>
-      <c r="E52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.97612098184230256</v>
-      </c>
-      <c r="F52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.92797896062899166</v>
-      </c>
-      <c r="G52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.8993022313141279</v>
-      </c>
-      <c r="H52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.88141899510200894</v>
-      </c>
-      <c r="I52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.86110504169926727</v>
-      </c>
-      <c r="J52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.85277713994202098</v>
-      </c>
-      <c r="K52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.84624542998719976</v>
-      </c>
-      <c r="L52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.8592497061727411</v>
-      </c>
-      <c r="M52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.84813020185023802</v>
-      </c>
-      <c r="N52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.84352939772612412</v>
-      </c>
-      <c r="O52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.84778383625724674</v>
-      </c>
-      <c r="P52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.83098196742300301</v>
-      </c>
-      <c r="Q52" s="7">
-        <f t="shared" si="65"/>
-        <v>0.75969065077472386</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53">
-        <f>(B$8*(1+B$21+B$26+B$27+B$28))*B$34</f>
-        <v>48507</v>
-      </c>
-      <c r="C53">
-        <f>(C$8*(1+C$21+C$26+C$27+C$28))*C$34</f>
-        <v>47936.393854748603</v>
-      </c>
-      <c r="D53">
-        <f>(D$8*(1+D$21+D$26+D$27+D$28))*D$34</f>
-        <v>48905.323350491344</v>
-      </c>
-      <c r="E53">
-        <f>(E$8*(1+E$21+E$26+E$27+E$28))*E$34</f>
-        <v>47207.083631484791</v>
-      </c>
-      <c r="F53">
-        <f>(F$8*(1+F$21+F$26+F$27+F$28))*F$34</f>
-        <v>44878.843112244896</v>
-      </c>
-      <c r="G53">
-        <f>(G$8*(1+G$21+G$26+G$27+G$28))*G$34</f>
-        <v>43491.981458590853</v>
-      </c>
-      <c r="H53">
-        <f>(H$8*(1+H$21+H$26+H$27+H$28))*H$34</f>
-        <v>42627.668132746898</v>
-      </c>
-      <c r="I53">
-        <f>(I$8*(1+I$21+I$26+I$27+I$28))*I$34</f>
-        <v>41645.233593749996</v>
-      </c>
-      <c r="J53">
-        <f>(J$8*(1+J$21+J$26+J$27+J$28))*J$34</f>
-        <v>41242.475048355896</v>
-      </c>
-      <c r="K53">
-        <f>(K$8*(1+K$21+K$26+K$27+K$28))*K$34</f>
-        <v>40926.588369441277</v>
-      </c>
-      <c r="L53">
-        <f>(L$8*(1+L$21+L$26+L$27+L$28))*L$34</f>
-        <v>45928.649324036691</v>
-      </c>
-      <c r="M53">
-        <f>(M$8*(1+M$21+M$26+M$27+M$28))*M$34</f>
-        <v>45333.184457386349</v>
-      </c>
-      <c r="N53">
-        <f>(N$8*(1+N$21+N$26+N$27+N$28))*N$34</f>
-        <v>45087.391776315788</v>
-      </c>
-      <c r="O53">
-        <f>(O$8*(1+O$21+O$26+O$27+O$28))*O$34</f>
-        <v>45313.981895598765</v>
-      </c>
-      <c r="P53">
-        <f>(P$8*(1+P$21+P$26+P$27+P$28))*P$34</f>
-        <v>44417.162276065566</v>
-      </c>
-      <c r="Q53">
-        <f>(Q$8*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
-        <v>40605.604155744928</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>43</v>
-      </c>
-      <c r="B54" s="7">
-        <f>B53/$B53</f>
-        <v>1</v>
-      </c>
-      <c r="C54" s="7">
-        <f t="shared" ref="C54:Q54" si="66">C53/$B53</f>
-        <v>0.98823662264721801</v>
-      </c>
-      <c r="D54" s="7">
-        <f t="shared" si="66"/>
-        <v>1.0082116673983414</v>
-      </c>
-      <c r="E54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.97320146847846267</v>
-      </c>
-      <c r="F54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.92520343686983109</v>
-      </c>
-      <c r="G54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.89661247775766084</v>
-      </c>
-      <c r="H54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.8787941561578102</v>
-      </c>
-      <c r="I54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.8585406970901106</v>
-      </c>
-      <c r="J54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.85023759557086398</v>
-      </c>
-      <c r="K54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.84372540807391261</v>
-      </c>
-      <c r="L54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.94684580213240754</v>
-      </c>
-      <c r="M54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.93456994778869751</v>
-      </c>
-      <c r="N54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.92950278879988013</v>
-      </c>
-      <c r="O54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.93417407581583611</v>
-      </c>
-      <c r="P54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.91568561807709337</v>
-      </c>
-      <c r="Q54" s="7">
-        <f t="shared" si="66"/>
-        <v>0.83710813193446154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55">
-        <f>(B$11*(1+B$21+B$26+B$27+B$28))*B$34</f>
-        <v>56119.5</v>
-      </c>
-      <c r="C55">
-        <f>(C$11*(1+C$21+C$26+C$27+C$28))*C$34</f>
-        <v>55308.782122905024</v>
-      </c>
-      <c r="D55">
-        <f>(D$11*(1+D$21+D$26+D$27+D$28))*D$34</f>
-        <v>56427.322882545624</v>
-      </c>
-      <c r="E55">
-        <f>(E$11*(1+E$21+E$26+E$27+E$28))*E$34</f>
-        <v>54468.112701252234</v>
-      </c>
-      <c r="F55">
-        <f>(F$11*(1+F$21+F$26+F$27+F$28))*F$34</f>
-        <v>51781.760204081635</v>
-      </c>
-      <c r="G55">
-        <f>(G$11*(1+G$21+G$26+G$27+G$28))*G$34</f>
-        <v>50181.58220024722</v>
-      </c>
-      <c r="H55">
-        <f>(H$11*(1+H$21+H$26+H$27+H$28))*H$34</f>
-        <v>49183.769292283083</v>
-      </c>
-      <c r="I55">
-        <f>(I$11*(1+I$21+I$26+I$27+I$28))*I$34</f>
-        <v>48050.237109374997</v>
-      </c>
-      <c r="J55">
-        <f>(J$11*(1+J$21+J$26+J$27+J$28))*J$34</f>
-        <v>47585.534622823987</v>
-      </c>
-      <c r="K55">
-        <f>(K$11*(1+K$21+K$26+K$27+K$28))*K$34</f>
-        <v>47221.174458380839</v>
-      </c>
-      <c r="L55">
-        <f>(L$11*(1+L$21+L$26+L$27+L$28))*L$34</f>
-        <v>45928.649324036691</v>
-      </c>
-      <c r="M55">
-        <f>(M$11*(1+M$21+M$26+M$27+M$28))*M$34</f>
-        <v>45333.184457386349</v>
-      </c>
-      <c r="N55">
-        <f>(N$11*(1+N$21+N$26+N$27+N$28))*N$34</f>
-        <v>45087.391776315788</v>
-      </c>
-      <c r="O55">
-        <f>(O$11*(1+O$21+O$26+O$27+O$28))*O$34</f>
-        <v>45313.981895598765</v>
-      </c>
-      <c r="P55">
-        <f>(P$11*(1+P$21+P$26+P$27+P$28))*P$34</f>
-        <v>47134.568689180327</v>
-      </c>
-      <c r="Q55">
-        <f>(Q$11*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
-        <v>46480.311885982948</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>43</v>
-      </c>
-      <c r="B56" s="7">
-        <f>B55/$B55</f>
-        <v>1</v>
-      </c>
-      <c r="C56" s="7">
-        <f t="shared" ref="C56:Q56" si="67">C55/$B55</f>
-        <v>0.98555372237644712</v>
-      </c>
-      <c r="D56" s="7">
-        <f t="shared" si="67"/>
-        <v>1.0054851323077652</v>
-      </c>
-      <c r="E56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.97057373464218732</v>
-      </c>
-      <c r="F56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.92270530215133129</v>
-      </c>
-      <c r="G56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.894191541269028</v>
-      </c>
-      <c r="H56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.87641139518853661</v>
-      </c>
-      <c r="I56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.85621285131505087</v>
-      </c>
-      <c r="J56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.84793226281103695</v>
-      </c>
-      <c r="K56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.84143968599828656</v>
-      </c>
-      <c r="L56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.81840802794103107</v>
-      </c>
-      <c r="M56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.80779736913882605</v>
-      </c>
-      <c r="N56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.80341756031888711</v>
-      </c>
-      <c r="O56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.80745519642189911</v>
-      </c>
-      <c r="P56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.83989644756600335</v>
-      </c>
-      <c r="Q56" s="7">
-        <f t="shared" si="67"/>
-        <v>0.82823816830126695</v>
+      <c r="C68" s="7">
+        <f t="shared" ref="C68:Q68" si="108">C67/$B67</f>
+        <v>1.0246705690535376</v>
+      </c>
+      <c r="D68" s="7">
+        <f t="shared" si="108"/>
+        <v>1.0400395584422526</v>
+      </c>
+      <c r="E68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.92685618871074993</v>
+      </c>
+      <c r="F68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.78782776040413749</v>
+      </c>
+      <c r="G68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.78782776040413749</v>
+      </c>
+      <c r="H68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.79570603800817885</v>
+      </c>
+      <c r="I68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.6365648304065431</v>
+      </c>
+      <c r="J68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.6365648304065431</v>
+      </c>
+      <c r="K68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.64293160131505089</v>
+      </c>
+      <c r="L68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.53972939887204974</v>
+      </c>
+      <c r="M68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.66062654157645739</v>
+      </c>
+      <c r="N68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.67384411835458258</v>
+      </c>
+      <c r="O68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.68731399246251301</v>
+      </c>
+      <c r="P68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.74395474300376874</v>
+      </c>
+      <c r="Q68" s="7">
+        <f t="shared" si="108"/>
+        <v>0.81853663699783485</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A37:XFD37">
+  <conditionalFormatting sqref="A38:XFD38">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:XFD40">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A42:XFD42">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44:XFD44">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A46:Q46">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:Q49">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -3661,7 +4498,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:XFD39">
+  <conditionalFormatting sqref="B51:Q51">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3673,7 +4510,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A41:XFD41">
+  <conditionalFormatting sqref="B53:Q53">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3685,7 +4522,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:XFD43">
+  <conditionalFormatting sqref="B55:Q55">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3697,7 +4534,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A45:Q45">
+  <conditionalFormatting sqref="B57:Q57">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -3709,7 +4546,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48:Q48">
+  <conditionalFormatting sqref="B60:Q60">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3721,7 +4558,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50:Q50">
+  <conditionalFormatting sqref="B62:Q62">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3733,7 +4570,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B52:Q52">
+  <conditionalFormatting sqref="B64:Q64">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3745,7 +4582,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:Q54">
+  <conditionalFormatting sqref="B66:Q66">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3757,7 +4594,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B56:Q56">
+  <conditionalFormatting sqref="B68:Q68">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Add CPIH Measure of Inflation
</commit_message>
<xml_diff>
--- a/Pay 2007-2022.xlsx
+++ b/Pay 2007-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelshaw/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelshaw/fpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAB8C29B-F4C1-CB49-B4D4-34D686DAAF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D3C7D1-FAFC-9941-B86A-C0A65B42E555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="0" windowWidth="20460" windowHeight="21000" xr2:uid="{E1BF444D-A2ED-614E-ACCD-35609FC30102}"/>
+    <workbookView xWindow="13140" yWindow="0" windowWidth="20460" windowHeight="21000" activeTab="3" xr2:uid="{E1BF444D-A2ED-614E-ACCD-35609FC30102}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>FY1</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>CT6 (2007, Freddo)</t>
+  </si>
+  <si>
+    <t>CPIH</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,6 +312,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -374,12 +383,12 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,10 +405,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -701,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3275042D-364E-CE44-842E-2AA03D01A8E4}">
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+    <sheetView zoomScale="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1682,32 +1687,24 @@
       <c r="K21">
         <v>0.5</v>
       </c>
-      <c r="L21" s="13">
-        <v>0</v>
-      </c>
-      <c r="M21" s="13">
-        <v>0</v>
-      </c>
-      <c r="N21" s="13">
-        <v>0</v>
-      </c>
-      <c r="O21" s="13">
-        <v>0</v>
-      </c>
-      <c r="P21" s="13">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1815,7 +1812,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2"/>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
@@ -1904,27 +1900,27 @@
         <v>0</v>
       </c>
       <c r="L27" s="1">
-        <f>L23/40</f>
+        <f t="shared" ref="L27:Q27" si="0">L23/40</f>
         <v>0.125</v>
       </c>
       <c r="M27" s="1">
-        <f>M23/40</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="N27" s="1">
-        <f>N23/40</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="O27" s="1">
-        <f>O23/40</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="P27" s="1">
-        <f>P23/40</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
       <c r="Q27" s="1">
-        <f>Q23/40</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
@@ -1963,31 +1959,30 @@
         <v>0</v>
       </c>
       <c r="L28" s="1">
-        <f>L24*(1/40)*0.37</f>
+        <f t="shared" ref="L28:Q28" si="1">L24*(1/40)*0.37</f>
         <v>0.11100000000000002</v>
       </c>
       <c r="M28" s="1">
-        <f>M24*(1/40)*0.37</f>
+        <f t="shared" si="1"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="N28" s="1">
-        <f>N24*(1/40)*0.37</f>
+        <f t="shared" si="1"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="O28" s="1">
-        <f>O24*(1/40)*0.37</f>
+        <f t="shared" si="1"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="P28" s="1">
-        <f>P24*(1/40)*0.37</f>
+        <f t="shared" si="1"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="Q28" s="1">
-        <f>Q24*(1/40)*0.37</f>
+        <f t="shared" si="1"/>
         <v>0.11100000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
@@ -2156,63 +2151,63 @@
         <v>1</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:Q33" si="0">$B$30/C30</f>
+        <f t="shared" ref="C33:Q33" si="2">$B$30/C30</f>
         <v>1</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.88235294117647045</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.74999999999999989</v>
       </c>
       <c r="G33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.74999999999999989</v>
       </c>
       <c r="H33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.74999999999999989</v>
       </c>
       <c r="I33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="J33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="K33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="L33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="M33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="N33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="O33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="P33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
     </row>
@@ -2221,67 +2216,67 @@
         <v>47</v>
       </c>
       <c r="B34">
-        <f>$B$31/B31</f>
+        <f t="shared" ref="B34:Q34" si="3">$B$31/B31</f>
         <v>1</v>
       </c>
       <c r="C34">
-        <f>$B$31/C31</f>
+        <f t="shared" si="3"/>
         <v>0.96576151121605658</v>
       </c>
       <c r="D34">
-        <f>$B$31/D31</f>
+        <f t="shared" si="3"/>
         <v>0.94457274826789839</v>
       </c>
       <c r="E34">
-        <f>$B$31/E31</f>
+        <f t="shared" si="3"/>
         <v>0.91498881431767332</v>
       </c>
       <c r="F34">
-        <f>$B$31/F31</f>
+        <f t="shared" si="3"/>
         <v>0.87580299785867233</v>
       </c>
       <c r="G34">
-        <f>$B$31/G31</f>
+        <f t="shared" si="3"/>
         <v>0.85119667013527578</v>
       </c>
       <c r="H34">
-        <f>$B$31/H31</f>
+        <f t="shared" si="3"/>
         <v>0.8304568527918782</v>
       </c>
       <c r="I34">
-        <f>$B$31/I31</f>
+        <f t="shared" si="3"/>
         <v>0.81799999999999995</v>
       </c>
       <c r="J34">
-        <f>$B$31/J31</f>
+        <f t="shared" si="3"/>
         <v>0.81799999999999995</v>
       </c>
       <c r="K34">
-        <f>$B$31/K31</f>
+        <f t="shared" si="3"/>
         <v>0.81231380337636538</v>
       </c>
       <c r="L34">
-        <f>$B$31/L31</f>
+        <f t="shared" si="3"/>
         <v>0.79110251450676972</v>
       </c>
       <c r="M34">
-        <f>$B$31/M31</f>
+        <f t="shared" si="3"/>
         <v>0.77242681775259669</v>
       </c>
       <c r="N34">
-        <f>$B$31/N31</f>
+        <f t="shared" si="3"/>
         <v>0.75881261595547311</v>
       </c>
       <c r="O34">
-        <f>$B$31/O31</f>
+        <f t="shared" si="3"/>
         <v>0.75252989880404775</v>
       </c>
       <c r="P34">
-        <f>$B$31/P31</f>
+        <f t="shared" si="3"/>
         <v>0.73297491039426521</v>
       </c>
       <c r="Q34">
-        <f>$B$31/Q31</f>
+        <f t="shared" si="3"/>
         <v>0.67214461791290059</v>
       </c>
     </row>
@@ -2290,137 +2285,136 @@
         <v>48</v>
       </c>
       <c r="B35">
-        <f>$B$32/B32</f>
+        <f t="shared" ref="B35:Q35" si="4">$B$32/B32</f>
         <v>1</v>
       </c>
       <c r="C35">
-        <f>$B$32/C32</f>
+        <f t="shared" si="4"/>
         <v>0.96182495344506513</v>
       </c>
       <c r="D35">
-        <f>$B$32/D32</f>
+        <f t="shared" si="4"/>
         <v>0.96677585400093591</v>
       </c>
       <c r="E35">
-        <f>$B$32/E32</f>
+        <f t="shared" si="4"/>
         <v>0.92397137745974955</v>
       </c>
       <c r="F35">
-        <f>$B$32/F32</f>
+        <f t="shared" si="4"/>
         <v>0.87840136054421769</v>
       </c>
       <c r="G35">
-        <f>$B$32/G32</f>
+        <f t="shared" si="4"/>
         <v>0.85125669550885874</v>
       </c>
       <c r="H35">
-        <f>$B$32/H32</f>
+        <f t="shared" si="4"/>
         <v>0.82606957217113153</v>
       </c>
       <c r="I35">
-        <f>$B$32/I32</f>
+        <f t="shared" si="4"/>
         <v>0.80703124999999998</v>
       </c>
       <c r="J35">
-        <f>$B$32/J32</f>
+        <f t="shared" si="4"/>
         <v>0.79922630560928432</v>
       </c>
       <c r="K35">
-        <f>$B$32/K32</f>
+        <f t="shared" si="4"/>
         <v>0.78525275560623331</v>
       </c>
       <c r="L35">
-        <f>$B$32/L32</f>
+        <f t="shared" si="4"/>
         <v>0.75816513761467885</v>
       </c>
       <c r="M35">
-        <f>$B$32/M32</f>
+        <f t="shared" si="4"/>
         <v>0.7336647727272726</v>
       </c>
       <c r="N35">
-        <f>$B$32/N32</f>
+        <f t="shared" si="4"/>
         <v>0.71537396121883656</v>
       </c>
       <c r="O35">
-        <f>$B$32/O32</f>
+        <f t="shared" si="4"/>
         <v>0.70487888092801088</v>
       </c>
       <c r="P35">
-        <f>$B$32/P32</f>
+        <f t="shared" si="4"/>
         <v>0.67737704918032782</v>
       </c>
       <c r="Q35">
-        <f>$B$32/Q32</f>
+        <f t="shared" si="4"/>
         <v>0.6071113723185424</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>41</v>
       </c>
       <c r="B37">
-        <f>(B$4*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <f t="shared" ref="B37:Q37" si="5">(B$4*(1+B$21+B$26+B$27+B$28))*B$34</f>
         <v>31578</v>
       </c>
       <c r="C37">
-        <f>(C$4*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <f t="shared" si="5"/>
         <v>31670.217237308145</v>
       </c>
       <c r="D37">
-        <f>(D$4*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <f t="shared" si="5"/>
         <v>31440.103926096999</v>
       </c>
       <c r="E37">
-        <f>(E$4*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <f t="shared" si="5"/>
         <v>30760.093959731541</v>
       </c>
       <c r="F37">
-        <f>(F$4*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <f t="shared" si="5"/>
         <v>29442.745182012848</v>
       </c>
       <c r="G37">
-        <f>(G$4*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <f t="shared" si="5"/>
         <v>28615.529656607701</v>
       </c>
       <c r="H37">
-        <f>(H$4*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <f t="shared" si="5"/>
         <v>28197.331979695431</v>
       </c>
       <c r="I37">
-        <f>(I$4*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <f t="shared" si="5"/>
         <v>27774.371999999999</v>
       </c>
       <c r="J37">
-        <f>(J$4*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <f t="shared" si="5"/>
         <v>27774.371999999999</v>
       </c>
       <c r="K37">
-        <f>(K$4*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <f t="shared" si="5"/>
         <v>27856.677259185697</v>
       </c>
       <c r="L37">
-        <f>(L$4*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <f t="shared" si="5"/>
         <v>27602.321442940032</v>
       </c>
       <c r="M37">
-        <f>(M$4*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <f t="shared" si="5"/>
         <v>27489.439195467414</v>
       </c>
       <c r="N37">
-        <f>(N$4*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <f t="shared" si="5"/>
         <v>27545.109667903522</v>
       </c>
       <c r="O37">
-        <f>(O$4*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <f t="shared" si="5"/>
         <v>27863.603232750684</v>
       </c>
       <c r="P37">
-        <f>(P$4*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <f t="shared" si="5"/>
         <v>27682.474537634407</v>
       </c>
       <c r="Q37">
-        <f>(Q$4*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <f t="shared" si="5"/>
         <v>25892.63996055875</v>
       </c>
     </row>
@@ -2433,63 +2427,63 @@
         <v>1</v>
       </c>
       <c r="C38" s="7">
-        <f t="shared" ref="C38" si="1">C37/$B37</f>
+        <f t="shared" ref="C38" si="6">C37/$B37</f>
         <v>1.0029203001237617</v>
       </c>
       <c r="D38" s="7">
-        <f t="shared" ref="D38" si="2">D37/$B37</f>
+        <f t="shared" ref="D38" si="7">D37/$B37</f>
         <v>0.99563315998787127</v>
       </c>
       <c r="E38" s="7">
-        <f t="shared" ref="E38" si="3">E37/$B37</f>
+        <f t="shared" ref="E38" si="8">E37/$B37</f>
         <v>0.97409886502411613</v>
       </c>
       <c r="F38" s="7">
-        <f t="shared" ref="F38" si="4">F37/$B37</f>
+        <f t="shared" ref="F38" si="9">F37/$B37</f>
         <v>0.93238156887747314</v>
       </c>
       <c r="G38" s="7">
-        <f t="shared" ref="G38" si="5">G37/$B37</f>
+        <f t="shared" ref="G38" si="10">G37/$B37</f>
         <v>0.90618562469465136</v>
       </c>
       <c r="H38" s="7">
-        <f t="shared" ref="H38" si="6">H37/$B37</f>
+        <f t="shared" ref="H38" si="11">H37/$B37</f>
         <v>0.89294230095938409</v>
       </c>
       <c r="I38" s="7">
-        <f t="shared" ref="I38" si="7">I37/$B37</f>
+        <f t="shared" ref="I38" si="12">I37/$B37</f>
         <v>0.87954816644499334</v>
       </c>
       <c r="J38" s="7">
-        <f t="shared" ref="J38" si="8">J37/$B37</f>
+        <f t="shared" ref="J38" si="13">J37/$B37</f>
         <v>0.87954816644499334</v>
       </c>
       <c r="K38" s="7">
-        <f t="shared" ref="K38" si="9">K37/$B37</f>
+        <f t="shared" ref="K38" si="14">K37/$B37</f>
         <v>0.88215457784488238</v>
       </c>
       <c r="L38" s="7">
-        <f t="shared" ref="L38" si="10">L37/$B37</f>
+        <f t="shared" ref="L38" si="15">L37/$B37</f>
         <v>0.87409973535182828</v>
       </c>
       <c r="M38" s="7">
-        <f t="shared" ref="M38" si="11">M37/$B37</f>
+        <f t="shared" ref="M38" si="16">M37/$B37</f>
         <v>0.87052502360717632</v>
       </c>
       <c r="N38" s="7">
-        <f t="shared" ref="N38" si="12">N37/$B37</f>
+        <f t="shared" ref="N38" si="17">N37/$B37</f>
         <v>0.87228797478952191</v>
       </c>
       <c r="O38" s="7">
-        <f t="shared" ref="O38" si="13">O37/$B37</f>
+        <f t="shared" ref="O38" si="18">O37/$B37</f>
         <v>0.88237390692097928</v>
       </c>
       <c r="P38" s="7">
-        <f t="shared" ref="P38" si="14">P37/$B37</f>
+        <f t="shared" ref="P38" si="19">P37/$B37</f>
         <v>0.8766379928315412</v>
       </c>
       <c r="Q38" s="7">
-        <f t="shared" ref="Q38" si="15">Q37/$B37</f>
+        <f t="shared" ref="Q38" si="20">Q37/$B37</f>
         <v>0.81995819749695198</v>
       </c>
     </row>
@@ -2498,67 +2492,67 @@
         <v>46</v>
       </c>
       <c r="B39">
-        <f>(B$5*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <f t="shared" ref="B39:Q39" si="21">(B$5*(1+B$21+B$26+B$27+B$28))*B$34</f>
         <v>39405</v>
       </c>
       <c r="C39">
-        <f>(C$5*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <f t="shared" si="21"/>
         <v>39281.383707201887</v>
       </c>
       <c r="D39">
-        <f>(D$5*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <f t="shared" si="21"/>
         <v>38996.213625866054</v>
       </c>
       <c r="E39">
-        <f>(E$5*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <f t="shared" si="21"/>
         <v>38152.288590604025</v>
       </c>
       <c r="F39">
-        <f>(F$5*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <f t="shared" si="21"/>
         <v>36518.357601713062</v>
       </c>
       <c r="G39">
-        <f>(G$5*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <f t="shared" si="21"/>
         <v>35492.347554630593</v>
       </c>
       <c r="H39">
-        <f>(H$5*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <f t="shared" si="21"/>
         <v>34973.85989847716</v>
       </c>
       <c r="I39">
-        <f>(I$5*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <f t="shared" si="21"/>
         <v>34449.252</v>
       </c>
       <c r="J39">
-        <f>(J$5*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <f t="shared" si="21"/>
         <v>34449.252</v>
       </c>
       <c r="K39">
-        <f>(K$5*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <f t="shared" si="21"/>
         <v>34552.173783515391</v>
       </c>
       <c r="L39">
-        <f>(L$5*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <f t="shared" si="21"/>
         <v>31948.95588974854</v>
       </c>
       <c r="M39">
-        <f>(M$5*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <f t="shared" si="21"/>
         <v>31819.537257790362</v>
       </c>
       <c r="N39">
-        <f>(N$5*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <f t="shared" si="21"/>
         <v>31883.447031539887</v>
       </c>
       <c r="O39">
-        <f>(O$5*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <f t="shared" si="21"/>
         <v>32251.851902483897</v>
       </c>
       <c r="P39">
-        <f>(P$5*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <f t="shared" si="21"/>
         <v>32042.214435483867</v>
       </c>
       <c r="Q39">
-        <f>(Q$5*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <f t="shared" si="21"/>
         <v>29970.748377978634</v>
       </c>
     </row>
@@ -2571,63 +2565,63 @@
         <v>1</v>
       </c>
       <c r="C40" s="7">
-        <f t="shared" ref="C40" si="16">C39/$B39</f>
+        <f t="shared" ref="C40" si="22">C39/$B39</f>
         <v>0.99686292874513105</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" ref="D40" si="17">D39/$B39</f>
+        <f t="shared" ref="D40" si="23">D39/$B39</f>
         <v>0.98962602781033004</v>
       </c>
       <c r="E40" s="7">
-        <f t="shared" ref="E40" si="18">E39/$B39</f>
+        <f t="shared" ref="E40" si="24">E39/$B39</f>
         <v>0.96820932852693886</v>
       </c>
       <c r="F40" s="7">
-        <f t="shared" ref="F40" si="19">F39/$B39</f>
+        <f t="shared" ref="F40" si="25">F39/$B39</f>
         <v>0.92674426092407214</v>
       </c>
       <c r="G40" s="7">
-        <f t="shared" ref="G40" si="20">G39/$B39</f>
+        <f t="shared" ref="G40" si="26">G39/$B39</f>
         <v>0.90070670104379125</v>
       </c>
       <c r="H40" s="7">
-        <f t="shared" ref="H40" si="21">H39/$B39</f>
+        <f t="shared" ref="H40" si="27">H39/$B39</f>
         <v>0.88754878564844963</v>
       </c>
       <c r="I40" s="7">
-        <f t="shared" ref="I40" si="22">I39/$B39</f>
+        <f t="shared" ref="I40" si="28">I39/$B39</f>
         <v>0.87423555386372287</v>
       </c>
       <c r="J40" s="7">
-        <f t="shared" ref="J40" si="23">J39/$B39</f>
+        <f t="shared" ref="J40" si="29">J39/$B39</f>
         <v>0.87423555386372287</v>
       </c>
       <c r="K40" s="7">
-        <f t="shared" ref="K40" si="24">K39/$B39</f>
+        <f t="shared" ref="K40" si="30">K39/$B39</f>
         <v>0.87684745041277479</v>
       </c>
       <c r="L40" s="7">
-        <f t="shared" ref="L40" si="25">L39/$B39</f>
+        <f t="shared" ref="L40" si="31">L39/$B39</f>
         <v>0.81078431391317196</v>
       </c>
       <c r="M40" s="7">
-        <f t="shared" ref="M40" si="26">M39/$B39</f>
+        <f t="shared" ref="M40" si="32">M39/$B39</f>
         <v>0.80749999385332727</v>
       </c>
       <c r="N40" s="7">
-        <f t="shared" ref="N40" si="27">N39/$B39</f>
+        <f t="shared" ref="N40" si="33">N39/$B39</f>
         <v>0.80912186350818138</v>
       </c>
       <c r="O40" s="7">
-        <f t="shared" ref="O40" si="28">O39/$B39</f>
+        <f t="shared" ref="O40" si="34">O39/$B39</f>
         <v>0.81847105449775148</v>
       </c>
       <c r="P40" s="7">
-        <f t="shared" ref="P40" si="29">P39/$B39</f>
+        <f t="shared" ref="P40" si="35">P39/$B39</f>
         <v>0.81315098174048639</v>
       </c>
       <c r="Q40" s="7">
-        <f t="shared" ref="Q40" si="30">Q39/$B39</f>
+        <f t="shared" ref="Q40" si="36">Q39/$B39</f>
         <v>0.76058237223648351</v>
       </c>
     </row>
@@ -2636,67 +2630,67 @@
         <v>61</v>
       </c>
       <c r="B41">
-        <f>(B$6*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <f t="shared" ref="B41:Q41" si="37">(B$6*(1+B$21+B$26+B$27+B$28))*B$34</f>
         <v>42177</v>
       </c>
       <c r="C41">
-        <f>(C$6*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <f t="shared" si="37"/>
         <v>41975.858323494685</v>
       </c>
       <c r="D41">
-        <f>(D$6*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <f t="shared" si="37"/>
         <v>41671.243648960743</v>
       </c>
       <c r="E41">
-        <f>(E$6*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <f t="shared" si="37"/>
         <v>40769.614093959732</v>
       </c>
       <c r="F41">
-        <f>(F$6*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <f t="shared" si="37"/>
         <v>39023.592077087793</v>
       </c>
       <c r="G41">
-        <f>(G$6*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <f t="shared" si="37"/>
         <v>37927.195629552552</v>
       </c>
       <c r="H41">
-        <f>(H$6*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <f t="shared" si="37"/>
         <v>37373.049746192897</v>
       </c>
       <c r="I41">
-        <f>(I$6*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <f t="shared" si="37"/>
         <v>36812.453999999998</v>
       </c>
       <c r="J41">
-        <f>(J$6*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <f t="shared" si="37"/>
         <v>36812.453999999998</v>
       </c>
       <c r="K41">
-        <f>(K$6*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <f t="shared" si="37"/>
         <v>36922.099304865937</v>
       </c>
       <c r="L41">
-        <f>(L$6*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <f t="shared" si="37"/>
         <v>37814.993692456475</v>
       </c>
       <c r="M41">
-        <f>(M$6*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <f t="shared" si="37"/>
         <v>37661.524096317276</v>
       </c>
       <c r="N41">
-        <f>(N$6*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <f t="shared" si="37"/>
         <v>37737.864684601111</v>
       </c>
       <c r="O41">
-        <f>(O$6*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <f t="shared" si="37"/>
         <v>38174.211786568529</v>
       </c>
       <c r="P41">
-        <f>(P$6*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <f t="shared" si="37"/>
         <v>37925.028553763441</v>
       </c>
       <c r="Q41">
-        <f>(Q$6*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <f t="shared" si="37"/>
         <v>35473.727433032043</v>
       </c>
     </row>
@@ -2709,63 +2703,63 @@
         <v>1</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" ref="C42:Q42" si="31">C41/$B41</f>
+        <f t="shared" ref="C42:Q42" si="38">C41/$B41</f>
         <v>0.99523101034911643</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.98800871681155</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.9666314364217401</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.92523394449789675</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.89923881806559391</v>
       </c>
       <c r="H42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.88610023819126293</v>
       </c>
       <c r="I42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.87280873461839381</v>
       </c>
       <c r="J42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.87280873461839381</v>
       </c>
       <c r="K42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.87540838146065236</v>
       </c>
       <c r="L42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.89657855448363977</v>
       </c>
       <c r="M42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.89293985101636619</v>
       </c>
       <c r="N42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.89474985619178959</v>
       </c>
       <c r="O42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.90509547351799624</v>
       </c>
       <c r="P42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.89918743755514718</v>
       </c>
       <c r="Q42" s="7">
-        <f t="shared" si="31"/>
+        <f t="shared" si="38"/>
         <v>0.84106805683268238</v>
       </c>
     </row>
@@ -2774,67 +2768,67 @@
         <v>60</v>
       </c>
       <c r="B43">
-        <f>(B$8*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <f t="shared" ref="B43:Q43" si="39">(B$8*(1+B$21+B$26+B$27+B$28))*B$34</f>
         <v>48507</v>
       </c>
       <c r="C43">
-        <f>(C$8*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <f t="shared" si="39"/>
         <v>48132.587957497046</v>
       </c>
       <c r="D43">
-        <f>(D$8*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <f t="shared" si="39"/>
         <v>47782.15704387991</v>
       </c>
       <c r="E43">
-        <f>(E$8*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <f t="shared" si="39"/>
         <v>46748.151006711407</v>
       </c>
       <c r="F43">
-        <f>(F$8*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <f t="shared" si="39"/>
         <v>44746.088865096361</v>
       </c>
       <c r="G43">
-        <f>(G$8*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <f t="shared" si="39"/>
         <v>43488.914672216444</v>
       </c>
       <c r="H43">
-        <f>(H$8*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <f t="shared" si="39"/>
         <v>42854.064974619294</v>
       </c>
       <c r="I43">
-        <f>(I$8*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <f t="shared" si="39"/>
         <v>42211.254000000001</v>
       </c>
       <c r="J43">
-        <f>(J$8*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <f t="shared" si="39"/>
         <v>42211.254000000001</v>
       </c>
       <c r="K43">
-        <f>(K$8*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <f t="shared" si="39"/>
         <v>42336.983118172786</v>
       </c>
       <c r="L43">
-        <f>(L$8*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <f t="shared" si="39"/>
         <v>47923.952402321069</v>
       </c>
       <c r="M43">
-        <f>(M$8*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <f t="shared" si="39"/>
         <v>47728.293235127472</v>
       </c>
       <c r="N43">
-        <f>(N$8*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <f t="shared" si="39"/>
         <v>47825.170547309834</v>
       </c>
       <c r="O43">
-        <f>(O$8*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <f t="shared" si="39"/>
         <v>48377.284570377175</v>
       </c>
       <c r="P43">
-        <f>(P$8*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <f t="shared" si="39"/>
         <v>48062.841188172039</v>
       </c>
       <c r="Q43">
-        <f>(Q$8*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <f t="shared" si="39"/>
         <v>44955.241385373869</v>
       </c>
     </row>
@@ -2847,63 +2841,63 @@
         <v>1</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" ref="C44:Q44" si="32">C43/$B43</f>
+        <f t="shared" ref="C44:Q44" si="40">C43/$B43</f>
         <v>0.992281278114438</v>
       </c>
       <c r="D44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.98505694114003983</v>
       </c>
       <c r="E44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.96374030566127378</v>
       </c>
       <c r="F44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.92246663090061976</v>
       </c>
       <c r="G44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.89654925417396347</v>
       </c>
       <c r="H44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.88346145864760328</v>
       </c>
       <c r="I44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.87020953676788915</v>
       </c>
       <c r="J44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.87020953676788915</v>
       </c>
       <c r="K44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.87280151561986485</v>
       </c>
       <c r="L44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.98798013487375158</v>
       </c>
       <c r="M44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.98394650741392942</v>
       </c>
       <c r="N44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.98594368951511813</v>
       </c>
       <c r="O44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.997325841020413</v>
       </c>
       <c r="P44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.99084340792405301</v>
       </c>
       <c r="Q44" s="7">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.9267784316773634</v>
       </c>
     </row>
@@ -2912,67 +2906,67 @@
         <v>59</v>
       </c>
       <c r="B45">
-        <f>(B$11*(1+B$21+B$26+B$27+B$28))*B$34</f>
+        <f t="shared" ref="B45:Q45" si="41">(B$11*(1+B$21+B$26+B$27+B$28))*B$34</f>
         <v>56119.5</v>
       </c>
       <c r="C45">
-        <f>(C$11*(1+C$21+C$26+C$27+C$28))*C$34</f>
+        <f t="shared" si="41"/>
         <v>55535.14994096812</v>
       </c>
       <c r="D45">
-        <f>(D$11*(1+D$21+D$26+D$27+D$28))*D$34</f>
+        <f t="shared" si="41"/>
         <v>55131.40531177829</v>
       </c>
       <c r="E45">
-        <f>(E$11*(1+E$21+E$26+E$27+E$28))*E$34</f>
+        <f t="shared" si="41"/>
         <v>53938.590604026846</v>
       </c>
       <c r="F45">
-        <f>(F$11*(1+F$21+F$26+F$27+F$28))*F$34</f>
+        <f t="shared" si="41"/>
         <v>51628.586723768734</v>
       </c>
       <c r="G45">
-        <f>(G$11*(1+G$21+G$26+G$27+G$28))*G$34</f>
+        <f t="shared" si="41"/>
         <v>50178.043704474505</v>
       </c>
       <c r="H45">
-        <f>(H$11*(1+H$21+H$26+H$27+H$28))*H$34</f>
+        <f t="shared" si="41"/>
         <v>49444.985786802034</v>
       </c>
       <c r="I45">
-        <f>(I$11*(1+I$21+I$26+I$27+I$28))*I$34</f>
+        <f t="shared" si="41"/>
         <v>48703.310999999994</v>
       </c>
       <c r="J45">
-        <f>(J$11*(1+J$21+J$26+J$27+J$28))*J$34</f>
+        <f t="shared" si="41"/>
         <v>48703.310999999994</v>
       </c>
       <c r="K45">
-        <f>(K$11*(1+K$21+K$26+K$27+K$28))*K$34</f>
+        <f t="shared" si="41"/>
         <v>48848.490566037734</v>
       </c>
       <c r="L45">
-        <f>(L$11*(1+L$21+L$26+L$27+L$28))*L$34</f>
+        <f t="shared" si="41"/>
         <v>47923.952402321069</v>
       </c>
       <c r="M45">
-        <f>(M$11*(1+M$21+M$26+M$27+M$28))*M$34</f>
+        <f t="shared" si="41"/>
         <v>47728.293235127472</v>
       </c>
       <c r="N45">
-        <f>(N$11*(1+N$21+N$26+N$27+N$28))*N$34</f>
+        <f t="shared" si="41"/>
         <v>47825.170547309834</v>
       </c>
       <c r="O45">
-        <f>(O$11*(1+O$21+O$26+O$27+O$28))*O$34</f>
+        <f t="shared" si="41"/>
         <v>48377.284570377175</v>
       </c>
       <c r="P45">
-        <f>(P$11*(1+P$21+P$26+P$27+P$28))*P$34</f>
+        <f t="shared" si="41"/>
         <v>51003.287317204296</v>
       </c>
       <c r="Q45">
-        <f>(Q$11*(1+Q$21+Q$26+Q$27+Q$28))*Q$34</f>
+        <f t="shared" si="41"/>
         <v>51459.242731306484</v>
       </c>
     </row>
@@ -2985,63 +2979,63 @@
         <v>1</v>
       </c>
       <c r="C46" s="7">
-        <f t="shared" ref="C46:Q46" si="33">C45/$B45</f>
+        <f t="shared" ref="C46:Q46" si="42">C45/$B45</f>
         <v>0.98958739726776113</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.98239302402513007</v>
       </c>
       <c r="E46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.9611381178383066</v>
       </c>
       <c r="F46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.91997588581097001</v>
       </c>
       <c r="G46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.89412848839484504</v>
       </c>
       <c r="H46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.88106604276235589</v>
       </c>
       <c r="I46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.86785005212092048</v>
       </c>
       <c r="J46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.86785005212092048</v>
       </c>
       <c r="K46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.87043702395847666</v>
       </c>
       <c r="L46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.85396256920181168</v>
       </c>
       <c r="M46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.85047609538801083</v>
       </c>
       <c r="N46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.85220236365808377</v>
       </c>
       <c r="O46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.86204054865736823</v>
       </c>
       <c r="P46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.90883360181762662</v>
       </c>
       <c r="Q46" s="7">
-        <f t="shared" si="33"/>
+        <f t="shared" si="42"/>
         <v>0.91695832520436715</v>
       </c>
     </row>
@@ -3050,67 +3044,67 @@
         <v>42</v>
       </c>
       <c r="B48">
-        <f>(B$4*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <f t="shared" ref="B48:Q48" si="43">(B$4*(1+B$21+B$26+B$27+B$28))*B$35</f>
         <v>31578</v>
       </c>
       <c r="C48">
-        <f>(C$4*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <f t="shared" si="43"/>
         <v>31541.12569832402</v>
       </c>
       <c r="D48">
-        <f>(D$4*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <f t="shared" si="43"/>
         <v>32179.134300421152</v>
       </c>
       <c r="E48">
-        <f>(E$4*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <f t="shared" si="43"/>
         <v>31062.069767441859</v>
       </c>
       <c r="F48">
-        <f>(F$4*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <f t="shared" si="43"/>
         <v>29530.09693877551</v>
       </c>
       <c r="G48">
-        <f>(G$4*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <f t="shared" si="43"/>
         <v>28617.547589616814</v>
       </c>
       <c r="H48">
-        <f>(H$4*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <f t="shared" si="43"/>
         <v>28048.3662534986</v>
       </c>
       <c r="I48">
-        <f>(I$4*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <f t="shared" si="43"/>
         <v>27401.939062499998</v>
       </c>
       <c r="J48">
-        <f>(J$4*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <f t="shared" si="43"/>
         <v>27136.929980657638</v>
       </c>
       <c r="K48">
-        <f>(K$4*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <f t="shared" si="43"/>
         <v>26928.672748004559</v>
       </c>
       <c r="L48">
-        <f>(L$4*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <f t="shared" si="43"/>
         <v>26453.104940917427</v>
       </c>
       <c r="M48">
-        <f>(M$4*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <f t="shared" si="43"/>
         <v>26109.9597997159</v>
       </c>
       <c r="N48">
-        <f>(N$4*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <f t="shared" si="43"/>
         <v>25968.274381578944</v>
       </c>
       <c r="O48">
-        <f>(O$4*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <f t="shared" si="43"/>
         <v>26099.249340839298</v>
       </c>
       <c r="P48">
-        <f>(P$4*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <f t="shared" si="43"/>
         <v>25582.694100983605</v>
       </c>
       <c r="Q48">
-        <f>(Q$4*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <f t="shared" si="43"/>
         <v>23387.401699676753</v>
       </c>
     </row>
@@ -3119,67 +3113,67 @@
         <v>43</v>
       </c>
       <c r="B49" s="7">
-        <f t="shared" ref="B49" si="34">B48/$B48</f>
+        <f t="shared" ref="B49" si="44">B48/$B48</f>
         <v>1</v>
       </c>
       <c r="C49" s="7">
-        <f t="shared" ref="C49" si="35">C48/$B48</f>
+        <f t="shared" ref="C49" si="45">C48/$B48</f>
         <v>0.99883227874862313</v>
       </c>
       <c r="D49" s="7">
-        <f t="shared" ref="D49" si="36">D48/$B48</f>
+        <f t="shared" ref="D49" si="46">D48/$B48</f>
         <v>1.0190364906080547</v>
       </c>
       <c r="E49" s="7">
-        <f t="shared" ref="E49" si="37">E48/$B48</f>
+        <f t="shared" ref="E49" si="47">E48/$B48</f>
         <v>0.9836617191539001</v>
       </c>
       <c r="F49" s="7">
-        <f t="shared" ref="F49" si="38">F48/$B48</f>
+        <f t="shared" ref="F49" si="48">F48/$B48</f>
         <v>0.9351477908282827</v>
       </c>
       <c r="G49" s="7">
-        <f t="shared" ref="G49" si="39">G48/$B48</f>
+        <f t="shared" ref="G49" si="49">G48/$B48</f>
         <v>0.9062495278237005</v>
       </c>
       <c r="H49" s="7">
-        <f t="shared" ref="H49" si="40">H48/$B48</f>
+        <f t="shared" ref="H49" si="50">H48/$B48</f>
         <v>0.88822491144146554</v>
       </c>
       <c r="I49" s="7">
-        <f t="shared" ref="I49" si="41">I48/$B48</f>
+        <f t="shared" ref="I49" si="51">I48/$B48</f>
         <v>0.86775410293558797</v>
       </c>
       <c r="J49" s="7">
-        <f t="shared" ref="J49" si="42">J48/$B48</f>
+        <f t="shared" ref="J49" si="52">J48/$B48</f>
         <v>0.8593618969110659</v>
       </c>
       <c r="K49" s="7">
-        <f t="shared" ref="K49" si="43">K48/$B48</f>
+        <f t="shared" ref="K49" si="53">K48/$B48</f>
         <v>0.85276688669341183</v>
       </c>
       <c r="L49" s="7">
-        <f t="shared" ref="L49" si="44">L48/$B48</f>
+        <f t="shared" ref="L49" si="54">L48/$B48</f>
         <v>0.83770678766601514</v>
       </c>
       <c r="M49" s="7">
-        <f t="shared" ref="M49" si="45">M48/$B48</f>
+        <f t="shared" ref="M49" si="55">M48/$B48</f>
         <v>0.82684019886363602</v>
       </c>
       <c r="N49" s="7">
-        <f t="shared" ref="N49" si="46">N48/$B48</f>
+        <f t="shared" ref="N49" si="56">N48/$B48</f>
         <v>0.82235335935078036</v>
       </c>
       <c r="O49" s="7">
-        <f t="shared" ref="O49" si="47">O48/$B48</f>
+        <f t="shared" ref="O49" si="57">O48/$B48</f>
         <v>0.82650102415730253</v>
       </c>
       <c r="P49" s="7">
-        <f t="shared" ref="P49" si="48">P48/$B48</f>
+        <f t="shared" ref="P49" si="58">P48/$B48</f>
         <v>0.81014295081967203</v>
       </c>
       <c r="Q49" s="7">
-        <f t="shared" ref="Q49" si="49">Q48/$B48</f>
+        <f t="shared" ref="Q49" si="59">Q48/$B48</f>
         <v>0.7406232725212728</v>
       </c>
     </row>
@@ -3188,67 +3182,67 @@
         <v>62</v>
       </c>
       <c r="B50">
-        <f>(B$5*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <f t="shared" ref="B50:Q50" si="60">(B$5*(1+B$21+B$26+B$27+B$28))*B$35</f>
         <v>39405</v>
       </c>
       <c r="C50">
-        <f>(C$5*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <f t="shared" si="60"/>
         <v>39121.26815642458</v>
       </c>
       <c r="D50">
-        <f>(D$5*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <f t="shared" si="60"/>
         <v>39912.857744501642</v>
       </c>
       <c r="E50">
-        <f>(E$5*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <f t="shared" si="60"/>
         <v>38526.834525939179</v>
       </c>
       <c r="F50">
-        <f>(F$5*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <f t="shared" si="60"/>
         <v>36626.701530612248</v>
       </c>
       <c r="G50">
-        <f>(G$5*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <f t="shared" si="60"/>
         <v>35494.850432632884</v>
       </c>
       <c r="H50">
-        <f>(H$5*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <f t="shared" si="60"/>
         <v>34789.093962415034</v>
       </c>
       <c r="I50">
-        <f>(I$5*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <f t="shared" si="60"/>
         <v>33987.314062500001</v>
       </c>
       <c r="J50">
-        <f>(J$5*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <f t="shared" si="60"/>
         <v>33658.616634429396</v>
       </c>
       <c r="K50">
-        <f>(K$5*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <f t="shared" si="60"/>
         <v>33401.118586088938</v>
       </c>
       <c r="L50">
-        <f>(L$5*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <f t="shared" si="60"/>
         <v>30618.768231192655</v>
       </c>
       <c r="M50">
-        <f>(M$5*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <f t="shared" si="60"/>
         <v>30222.764194602267</v>
       </c>
       <c r="N50">
-        <f>(N$5*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <f t="shared" si="60"/>
         <v>30058.261184210522</v>
       </c>
       <c r="O50">
-        <f>(O$5*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <f t="shared" si="60"/>
         <v>30209.629295803476</v>
       </c>
       <c r="P50">
-        <f>(P$5*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <f t="shared" si="60"/>
         <v>29611.737531147537</v>
       </c>
       <c r="Q50">
-        <f>(Q$5*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <f t="shared" si="60"/>
         <v>27070.933385836022</v>
       </c>
     </row>
@@ -3257,67 +3251,67 @@
         <v>43</v>
       </c>
       <c r="B51" s="7">
-        <f t="shared" ref="B51" si="50">B50/$B50</f>
+        <f t="shared" ref="B51" si="61">B50/$B50</f>
         <v>1</v>
       </c>
       <c r="C51" s="7">
-        <f t="shared" ref="C51" si="51">C50/$B50</f>
+        <f t="shared" ref="C51" si="62">C50/$B50</f>
         <v>0.99279959792982053</v>
       </c>
       <c r="D51" s="7">
-        <f t="shared" ref="D51" si="52">D50/$B50</f>
+        <f t="shared" ref="D51" si="63">D50/$B50</f>
         <v>1.0128881549169304</v>
       </c>
       <c r="E51" s="7">
-        <f t="shared" ref="E51" si="53">E50/$B50</f>
+        <f t="shared" ref="E51" si="64">E50/$B50</f>
         <v>0.97771436431770531</v>
       </c>
       <c r="F51" s="7">
-        <f t="shared" ref="F51" si="54">F50/$B50</f>
+        <f t="shared" ref="F51" si="65">F50/$B50</f>
         <v>0.92949375791428113</v>
       </c>
       <c r="G51" s="7">
-        <f t="shared" ref="G51" si="55">G50/$B50</f>
+        <f t="shared" ref="G51" si="66">G50/$B50</f>
         <v>0.90077021780568156</v>
       </c>
       <c r="H51" s="7">
-        <f t="shared" ref="H51" si="56">H50/$B50</f>
+        <f t="shared" ref="H51" si="67">H50/$B50</f>
         <v>0.88285988992298015</v>
       </c>
       <c r="I51" s="7">
-        <f t="shared" ref="I51" si="57">I50/$B50</f>
+        <f t="shared" ref="I51" si="68">I50/$B50</f>
         <v>0.86251272839741155</v>
       </c>
       <c r="J51" s="7">
-        <f t="shared" ref="J51" si="58">J50/$B50</f>
+        <f t="shared" ref="J51" si="69">J50/$B50</f>
         <v>0.85417121264888707</v>
       </c>
       <c r="K51" s="7">
-        <f t="shared" ref="K51" si="59">K50/$B50</f>
+        <f t="shared" ref="K51" si="70">K50/$B50</f>
         <v>0.84763655845930563</v>
       </c>
       <c r="L51" s="7">
-        <f t="shared" ref="L51" si="60">L50/$B50</f>
+        <f t="shared" ref="L51" si="71">L50/$B50</f>
         <v>0.77702748968893931</v>
       </c>
       <c r="M51" s="7">
-        <f t="shared" ref="M51" si="61">M50/$B50</f>
+        <f t="shared" ref="M51" si="72">M50/$B50</f>
         <v>0.76697790114458231</v>
       </c>
       <c r="N51" s="7">
-        <f t="shared" ref="N51" si="62">N50/$B50</f>
+        <f t="shared" ref="N51" si="73">N50/$B50</f>
         <v>0.76280322761605179</v>
       </c>
       <c r="O51" s="7">
-        <f t="shared" ref="O51" si="63">O50/$B50</f>
+        <f t="shared" ref="O51" si="74">O50/$B50</f>
         <v>0.76664457037948164</v>
       </c>
       <c r="P51" s="7">
-        <f t="shared" ref="P51" si="64">P50/$B50</f>
+        <f t="shared" ref="P51" si="75">P50/$B50</f>
         <v>0.75147157800146014</v>
       </c>
       <c r="Q51" s="7">
-        <f t="shared" ref="Q51" si="65">Q50/$B50</f>
+        <f t="shared" ref="Q51" si="76">Q50/$B50</f>
         <v>0.68699234578951962</v>
       </c>
     </row>
@@ -3326,67 +3320,67 @@
         <v>63</v>
       </c>
       <c r="B52">
-        <f>(B$6*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <f t="shared" ref="B52:Q52" si="77">(B$6*(1+B$21+B$26+B$27+B$28))*B$35</f>
         <v>42177</v>
       </c>
       <c r="C52">
-        <f>(C$6*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <f t="shared" si="77"/>
         <v>41804.75977653631</v>
       </c>
       <c r="D52">
-        <f>(D$6*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <f t="shared" si="77"/>
         <v>42650.766963032293</v>
       </c>
       <c r="E52">
-        <f>(E$6*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <f t="shared" si="77"/>
         <v>41169.854651162794</v>
       </c>
       <c r="F52">
-        <f>(F$6*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <f t="shared" si="77"/>
         <v>39139.368622448979</v>
       </c>
       <c r="G52">
-        <f>(G$6*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <f t="shared" si="77"/>
         <v>37929.870210135974</v>
       </c>
       <c r="H52">
-        <f>(H$6*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <f t="shared" si="77"/>
         <v>37175.608956417433</v>
       </c>
       <c r="I52">
-        <f>(I$6*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <f t="shared" si="77"/>
         <v>36318.827343749996</v>
       </c>
       <c r="J52">
-        <f>(J$6*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <f t="shared" si="77"/>
         <v>35967.58143133462</v>
       </c>
       <c r="K52">
-        <f>(K$6*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <f t="shared" si="77"/>
         <v>35692.093500570125</v>
       </c>
       <c r="L52">
-        <f>(L$6*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <f t="shared" si="77"/>
         <v>36240.574857247702</v>
       </c>
       <c r="M52">
-        <f>(M$6*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <f t="shared" si="77"/>
         <v>35771.587523437491</v>
       </c>
       <c r="N52">
-        <f>(N$6*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <f t="shared" si="77"/>
         <v>35577.539407894736</v>
       </c>
       <c r="O52">
-        <f>(O$6*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <f t="shared" si="77"/>
         <v>35756.978861821895</v>
       </c>
       <c r="P52">
-        <f>(P$6*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <f t="shared" si="77"/>
         <v>35048.326439999997</v>
       </c>
       <c r="Q52">
-        <f>(Q$6*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <f t="shared" si="77"/>
         <v>32041.47257772553</v>
       </c>
     </row>
@@ -3399,63 +3393,63 @@
         <v>1</v>
       </c>
       <c r="C53" s="7">
-        <f t="shared" ref="C53:Q53" si="66">C52/$B52</f>
+        <f t="shared" ref="C53:Q53" si="78">C52/$B52</f>
         <v>0.99117433142557099</v>
       </c>
       <c r="D53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>1.0112328274422622</v>
       </c>
       <c r="E53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.97612098184230256</v>
       </c>
       <c r="F53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.92797896062899166</v>
       </c>
       <c r="G53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.8993022313141279</v>
       </c>
       <c r="H53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.88141899510200894</v>
       </c>
       <c r="I53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.86110504169926727</v>
       </c>
       <c r="J53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.85277713994202098</v>
       </c>
       <c r="K53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.84624542998719976</v>
       </c>
       <c r="L53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.8592497061727411</v>
       </c>
       <c r="M53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.84813020185023802</v>
       </c>
       <c r="N53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.84352939772612412</v>
       </c>
       <c r="O53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.84778383625724674</v>
       </c>
       <c r="P53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.83098196742300301</v>
       </c>
       <c r="Q53" s="7">
-        <f t="shared" si="66"/>
+        <f t="shared" si="78"/>
         <v>0.75969065077472386</v>
       </c>
     </row>
@@ -3464,67 +3458,67 @@
         <v>64</v>
       </c>
       <c r="B54">
-        <f>(B$8*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <f t="shared" ref="B54:Q54" si="79">(B$8*(1+B$21+B$26+B$27+B$28))*B$35</f>
         <v>48507</v>
       </c>
       <c r="C54">
-        <f>(C$8*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <f t="shared" si="79"/>
         <v>47936.393854748603</v>
       </c>
       <c r="D54">
-        <f>(D$8*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <f t="shared" si="79"/>
         <v>48905.323350491344</v>
       </c>
       <c r="E54">
-        <f>(E$8*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <f t="shared" si="79"/>
         <v>47207.083631484791</v>
       </c>
       <c r="F54">
-        <f>(F$8*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <f t="shared" si="79"/>
         <v>44878.843112244896</v>
       </c>
       <c r="G54">
-        <f>(G$8*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <f t="shared" si="79"/>
         <v>43491.981458590853</v>
       </c>
       <c r="H54">
-        <f>(H$8*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <f t="shared" si="79"/>
         <v>42627.668132746898</v>
       </c>
       <c r="I54">
-        <f>(I$8*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <f t="shared" si="79"/>
         <v>41645.233593749996</v>
       </c>
       <c r="J54">
-        <f>(J$8*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <f t="shared" si="79"/>
         <v>41242.475048355896</v>
       </c>
       <c r="K54">
-        <f>(K$8*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <f t="shared" si="79"/>
         <v>40926.588369441277</v>
       </c>
       <c r="L54">
-        <f>(L$8*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <f t="shared" si="79"/>
         <v>45928.649324036691</v>
       </c>
       <c r="M54">
-        <f>(M$8*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <f t="shared" si="79"/>
         <v>45333.184457386349</v>
       </c>
       <c r="N54">
-        <f>(N$8*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <f t="shared" si="79"/>
         <v>45087.391776315788</v>
       </c>
       <c r="O54">
-        <f>(O$8*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <f t="shared" si="79"/>
         <v>45313.981895598765</v>
       </c>
       <c r="P54">
-        <f>(P$8*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <f t="shared" si="79"/>
         <v>44417.162276065566</v>
       </c>
       <c r="Q54">
-        <f>(Q$8*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <f t="shared" si="79"/>
         <v>40605.604155744928</v>
       </c>
     </row>
@@ -3537,63 +3531,63 @@
         <v>1</v>
       </c>
       <c r="C55" s="7">
-        <f t="shared" ref="C55:Q55" si="67">C54/$B54</f>
+        <f t="shared" ref="C55:Q55" si="80">C54/$B54</f>
         <v>0.98823662264721801</v>
       </c>
       <c r="D55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>1.0082116673983414</v>
       </c>
       <c r="E55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.97320146847846267</v>
       </c>
       <c r="F55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.92520343686983109</v>
       </c>
       <c r="G55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.89661247775766084</v>
       </c>
       <c r="H55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.8787941561578102</v>
       </c>
       <c r="I55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.8585406970901106</v>
       </c>
       <c r="J55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.85023759557086398</v>
       </c>
       <c r="K55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.84372540807391261</v>
       </c>
       <c r="L55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.94684580213240754</v>
       </c>
       <c r="M55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.93456994778869751</v>
       </c>
       <c r="N55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.92950278879988013</v>
       </c>
       <c r="O55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.93417407581583611</v>
       </c>
       <c r="P55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.91568561807709337</v>
       </c>
       <c r="Q55" s="7">
-        <f t="shared" si="67"/>
+        <f t="shared" si="80"/>
         <v>0.83710813193446154</v>
       </c>
     </row>
@@ -3602,67 +3596,67 @@
         <v>65</v>
       </c>
       <c r="B56">
-        <f>(B$11*(1+B$21+B$26+B$27+B$28))*B$35</f>
+        <f t="shared" ref="B56:Q56" si="81">(B$11*(1+B$21+B$26+B$27+B$28))*B$35</f>
         <v>56119.5</v>
       </c>
       <c r="C56">
-        <f>(C$11*(1+C$21+C$26+C$27+C$28))*C$35</f>
+        <f t="shared" si="81"/>
         <v>55308.782122905024</v>
       </c>
       <c r="D56">
-        <f>(D$11*(1+D$21+D$26+D$27+D$28))*D$35</f>
+        <f t="shared" si="81"/>
         <v>56427.322882545624</v>
       </c>
       <c r="E56">
-        <f>(E$11*(1+E$21+E$26+E$27+E$28))*E$35</f>
+        <f t="shared" si="81"/>
         <v>54468.112701252234</v>
       </c>
       <c r="F56">
-        <f>(F$11*(1+F$21+F$26+F$27+F$28))*F$35</f>
+        <f t="shared" si="81"/>
         <v>51781.760204081635</v>
       </c>
       <c r="G56">
-        <f>(G$11*(1+G$21+G$26+G$27+G$28))*G$35</f>
+        <f t="shared" si="81"/>
         <v>50181.58220024722</v>
       </c>
       <c r="H56">
-        <f>(H$11*(1+H$21+H$26+H$27+H$28))*H$35</f>
+        <f t="shared" si="81"/>
         <v>49183.769292283083</v>
       </c>
       <c r="I56">
-        <f>(I$11*(1+I$21+I$26+I$27+I$28))*I$35</f>
+        <f t="shared" si="81"/>
         <v>48050.237109374997</v>
       </c>
       <c r="J56">
-        <f>(J$11*(1+J$21+J$26+J$27+J$28))*J$35</f>
+        <f t="shared" si="81"/>
         <v>47585.534622823987</v>
       </c>
       <c r="K56">
-        <f>(K$11*(1+K$21+K$26+K$27+K$28))*K$35</f>
+        <f t="shared" si="81"/>
         <v>47221.174458380839</v>
       </c>
       <c r="L56">
-        <f>(L$11*(1+L$21+L$26+L$27+L$28))*L$35</f>
+        <f t="shared" si="81"/>
         <v>45928.649324036691</v>
       </c>
       <c r="M56">
-        <f>(M$11*(1+M$21+M$26+M$27+M$28))*M$35</f>
+        <f t="shared" si="81"/>
         <v>45333.184457386349</v>
       </c>
       <c r="N56">
-        <f>(N$11*(1+N$21+N$26+N$27+N$28))*N$35</f>
+        <f t="shared" si="81"/>
         <v>45087.391776315788</v>
       </c>
       <c r="O56">
-        <f>(O$11*(1+O$21+O$26+O$27+O$28))*O$35</f>
+        <f t="shared" si="81"/>
         <v>45313.981895598765</v>
       </c>
       <c r="P56">
-        <f>(P$11*(1+P$21+P$26+P$27+P$28))*P$35</f>
+        <f t="shared" si="81"/>
         <v>47134.568689180327</v>
       </c>
       <c r="Q56">
-        <f>(Q$11*(1+Q$21+Q$26+Q$27+Q$28))*Q$35</f>
+        <f t="shared" si="81"/>
         <v>46480.311885982948</v>
       </c>
     </row>
@@ -3675,63 +3669,63 @@
         <v>1</v>
       </c>
       <c r="C57" s="7">
-        <f t="shared" ref="C57:Q57" si="68">C56/$B56</f>
+        <f t="shared" ref="C57:Q57" si="82">C56/$B56</f>
         <v>0.98555372237644712</v>
       </c>
       <c r="D57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>1.0054851323077652</v>
       </c>
       <c r="E57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.97057373464218732</v>
       </c>
       <c r="F57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.92270530215133129</v>
       </c>
       <c r="G57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.894191541269028</v>
       </c>
       <c r="H57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.87641139518853661</v>
       </c>
       <c r="I57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.85621285131505087</v>
       </c>
       <c r="J57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.84793226281103695</v>
       </c>
       <c r="K57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.84143968599828656</v>
       </c>
       <c r="L57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.81840802794103107</v>
       </c>
       <c r="M57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.80779736913882605</v>
       </c>
       <c r="N57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.80341756031888711</v>
       </c>
       <c r="O57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.80745519642189911</v>
       </c>
       <c r="P57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.83989644756600335</v>
       </c>
       <c r="Q57" s="7">
-        <f t="shared" si="68"/>
+        <f t="shared" si="82"/>
         <v>0.82823816830126695</v>
       </c>
     </row>
@@ -3744,63 +3738,63 @@
         <v>31578</v>
       </c>
       <c r="C59">
-        <f t="shared" ref="C59:Q59" si="69">(C$4*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <f t="shared" ref="C59:Q59" si="83">(C$4*(1+C$21+C$26+C$27+C$28))*C$33</f>
         <v>32793</v>
       </c>
       <c r="D59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>33285</v>
       </c>
       <c r="E59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>29662.941176470584</v>
       </c>
       <c r="F59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>25213.499999999996</v>
       </c>
       <c r="G59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>25213.499999999996</v>
       </c>
       <c r="H59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>25465.499999999996</v>
       </c>
       <c r="I59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>20372.399999999998</v>
       </c>
       <c r="J59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>20372.399999999998</v>
       </c>
       <c r="K59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>20575.8</v>
       </c>
       <c r="L59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>17445.476999999999</v>
       </c>
       <c r="M59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>21353.043599999997</v>
       </c>
       <c r="N59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>21780.167399999995</v>
       </c>
       <c r="O59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>22215.943799999997</v>
       </c>
       <c r="P59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>22660.372800000001</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="69"/>
+        <f t="shared" si="83"/>
         <v>23113.454399999999</v>
       </c>
     </row>
@@ -3809,67 +3803,67 @@
         <v>43</v>
       </c>
       <c r="B60" s="7">
-        <f t="shared" ref="B60" si="70">B59/$B59</f>
+        <f t="shared" ref="B60" si="84">B59/$B59</f>
         <v>1</v>
       </c>
       <c r="C60" s="7">
-        <f t="shared" ref="C60" si="71">C59/$B59</f>
+        <f t="shared" ref="C60" si="85">C59/$B59</f>
         <v>1.0384761542846286</v>
       </c>
       <c r="D60" s="7">
-        <f t="shared" ref="D60" si="72">D59/$B59</f>
+        <f t="shared" ref="D60" si="86">D59/$B59</f>
         <v>1.0540566216986509</v>
       </c>
       <c r="E60" s="7">
-        <f t="shared" ref="E60" si="73">E59/$B59</f>
+        <f t="shared" ref="E60" si="87">E59/$B59</f>
         <v>0.93935465122777195</v>
       </c>
       <c r="F60" s="7">
-        <f t="shared" ref="F60" si="74">F59/$B59</f>
+        <f t="shared" ref="F60" si="88">F59/$B59</f>
         <v>0.79845145354360614</v>
       </c>
       <c r="G60" s="7">
-        <f t="shared" ref="G60" si="75">G59/$B59</f>
+        <f t="shared" ref="G60" si="89">G59/$B59</f>
         <v>0.79845145354360614</v>
       </c>
       <c r="H60" s="7">
-        <f t="shared" ref="H60" si="76">H59/$B59</f>
+        <f t="shared" ref="H60" si="90">H59/$B59</f>
         <v>0.80643169295078843</v>
       </c>
       <c r="I60" s="7">
-        <f t="shared" ref="I60" si="77">I59/$B59</f>
+        <f t="shared" ref="I60" si="91">I59/$B59</f>
         <v>0.6451453543606307</v>
       </c>
       <c r="J60" s="7">
-        <f t="shared" ref="J60" si="78">J59/$B59</f>
+        <f t="shared" ref="J60" si="92">J59/$B59</f>
         <v>0.6451453543606307</v>
       </c>
       <c r="K60" s="7">
-        <f t="shared" ref="K60" si="79">K59/$B59</f>
+        <f t="shared" ref="K60" si="93">K59/$B59</f>
         <v>0.65158654759642787</v>
       </c>
       <c r="L60" s="7">
-        <f t="shared" ref="L60" si="80">L59/$B59</f>
+        <f t="shared" ref="L60" si="94">L59/$B59</f>
         <v>0.55245667870036097</v>
       </c>
       <c r="M60" s="7">
-        <f t="shared" ref="M60" si="81">M59/$B59</f>
+        <f t="shared" ref="M60" si="95">M59/$B59</f>
         <v>0.67619999999999991</v>
       </c>
       <c r="N60" s="7">
-        <f t="shared" ref="N60" si="82">N59/$B59</f>
+        <f t="shared" ref="N60" si="96">N59/$B59</f>
         <v>0.68972599277978319</v>
       </c>
       <c r="O60" s="7">
-        <f t="shared" ref="O60" si="83">O59/$B59</f>
+        <f t="shared" ref="O60" si="97">O59/$B59</f>
         <v>0.70352599277978334</v>
       </c>
       <c r="P60" s="7">
-        <f t="shared" ref="P60" si="84">P59/$B59</f>
+        <f t="shared" ref="P60" si="98">P59/$B59</f>
         <v>0.71760000000000002</v>
       </c>
       <c r="Q60" s="7">
-        <f t="shared" ref="Q60" si="85">Q59/$B59</f>
+        <f t="shared" ref="Q60" si="99">Q59/$B59</f>
         <v>0.73194801444043323</v>
       </c>
     </row>
@@ -3882,63 +3876,63 @@
         <v>39405</v>
       </c>
       <c r="C61">
-        <f t="shared" ref="C61:Q61" si="86">(C$5*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <f t="shared" ref="C61:Q61" si="100">(C$5*(1+C$21+C$26+C$27+C$28))*C$33</f>
         <v>40674</v>
       </c>
       <c r="D61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>41284.5</v>
       </c>
       <c r="E61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>36791.470588235286</v>
       </c>
       <c r="F61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>31272.749999999996</v>
       </c>
       <c r="G61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>31272.749999999996</v>
       </c>
       <c r="H61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>31585.499999999996</v>
       </c>
       <c r="I61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>25268.399999999998</v>
       </c>
       <c r="J61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>25268.399999999998</v>
       </c>
       <c r="K61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>25521.3</v>
       </c>
       <c r="L61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>20192.677499999998</v>
       </c>
       <c r="M61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>24716.545199999997</v>
       </c>
       <c r="N61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>25210.529999999995</v>
       </c>
       <c r="O61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>25714.740599999997</v>
       </c>
       <c r="P61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>26229.177</v>
       </c>
       <c r="Q61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="100"/>
         <v>26753.839199999999</v>
       </c>
     </row>
@@ -3947,67 +3941,67 @@
         <v>43</v>
       </c>
       <c r="B62" s="7">
-        <f t="shared" ref="B62" si="87">B61/$B61</f>
+        <f t="shared" ref="B62" si="101">B61/$B61</f>
         <v>1</v>
       </c>
       <c r="C62" s="7">
-        <f t="shared" ref="C62" si="88">C61/$B61</f>
+        <f t="shared" ref="C62" si="102">C61/$B61</f>
         <v>1.0322040350209365</v>
       </c>
       <c r="D62" s="7">
-        <f t="shared" ref="D62" si="89">D61/$B61</f>
+        <f t="shared" ref="D62" si="103">D61/$B61</f>
         <v>1.0476969927674153</v>
       </c>
       <c r="E62" s="7">
-        <f t="shared" ref="E62" si="90">E61/$B61</f>
+        <f t="shared" ref="E62" si="104">E61/$B61</f>
         <v>0.93367518305380759</v>
       </c>
       <c r="F62" s="7">
-        <f t="shared" ref="F62" si="91">F61/$B61</f>
+        <f t="shared" ref="F62" si="105">F61/$B61</f>
         <v>0.79362390559573648</v>
       </c>
       <c r="G62" s="7">
-        <f t="shared" ref="G62" si="92">G61/$B61</f>
+        <f t="shared" ref="G62" si="106">G61/$B61</f>
         <v>0.79362390559573648</v>
       </c>
       <c r="H62" s="7">
-        <f t="shared" ref="H62" si="93">H61/$B61</f>
+        <f t="shared" ref="H62" si="107">H61/$B61</f>
         <v>0.80156071564522258</v>
       </c>
       <c r="I62" s="7">
-        <f t="shared" ref="I62" si="94">I61/$B61</f>
+        <f t="shared" ref="I62" si="108">I61/$B61</f>
         <v>0.64124857251617806</v>
       </c>
       <c r="J62" s="7">
-        <f t="shared" ref="J62" si="95">J61/$B61</f>
+        <f t="shared" ref="J62" si="109">J61/$B61</f>
         <v>0.64124857251617806</v>
       </c>
       <c r="K62" s="7">
-        <f t="shared" ref="K62" si="96">K61/$B61</f>
+        <f t="shared" ref="K62" si="110">K61/$B61</f>
         <v>0.64766653977921584</v>
       </c>
       <c r="L62" s="7">
-        <f t="shared" ref="L62" si="97">L61/$B61</f>
+        <f t="shared" ref="L62" si="111">L61/$B61</f>
         <v>0.51243947468595352</v>
       </c>
       <c r="M62" s="7">
-        <f t="shared" ref="M62" si="98">M61/$B61</f>
+        <f t="shared" ref="M62" si="112">M61/$B61</f>
         <v>0.6272438827559953</v>
       </c>
       <c r="N62" s="7">
-        <f t="shared" ref="N62" si="99">N61/$B61</f>
+        <f t="shared" ref="N62" si="113">N61/$B61</f>
         <v>0.63977997716025869</v>
       </c>
       <c r="O62" s="7">
-        <f t="shared" ref="O62" si="100">O61/$B61</f>
+        <f t="shared" ref="O62" si="114">O61/$B61</f>
         <v>0.652575576703464</v>
       </c>
       <c r="P62" s="7">
-        <f t="shared" ref="P62" si="101">P61/$B61</f>
+        <f t="shared" ref="P62" si="115">P61/$B61</f>
         <v>0.66563068138561099</v>
       </c>
       <c r="Q62" s="7">
-        <f t="shared" ref="Q62" si="102">Q61/$B61</f>
+        <f t="shared" ref="Q62" si="116">Q61/$B61</f>
         <v>0.67894529120669966</v>
       </c>
     </row>
@@ -4020,63 +4014,63 @@
         <v>42177</v>
       </c>
       <c r="C63">
-        <f t="shared" ref="C63:Q63" si="103">(C$6*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <f t="shared" ref="C63:Q63" si="117">(C$6*(1+C$21+C$26+C$27+C$28))*C$33</f>
         <v>43464</v>
       </c>
       <c r="D63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>44116.5</v>
       </c>
       <c r="E63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>39315.44117647058</v>
       </c>
       <c r="F63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>33418.124999999993</v>
       </c>
       <c r="G63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>33418.124999999993</v>
       </c>
       <c r="H63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>33752.249999999993</v>
       </c>
       <c r="I63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>27001.8</v>
       </c>
       <c r="J63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>27001.8</v>
       </c>
       <c r="K63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>27271.8</v>
       </c>
       <c r="L63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>23900.1855</v>
       </c>
       <c r="M63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>29254.440599999998</v>
       </c>
       <c r="N63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>29839.670999999995</v>
       </c>
       <c r="O63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>30436.700399999994</v>
       </c>
       <c r="P63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>31044.742200000001</v>
       </c>
       <c r="Q63">
-        <f t="shared" si="103"/>
+        <f t="shared" si="117"/>
         <v>31666.156199999998</v>
       </c>
     </row>
@@ -4089,63 +4083,63 @@
         <v>1</v>
       </c>
       <c r="C64" s="7">
-        <f t="shared" ref="C64:Q64" si="104">C63/$B63</f>
+        <f t="shared" ref="C64:Q64" si="118">C63/$B63</f>
         <v>1.0305142613272638</v>
       </c>
       <c r="D64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>1.0459847784337435</v>
       </c>
       <c r="E64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.93215357129408394</v>
       </c>
       <c r="F64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.79233053559997135</v>
       </c>
       <c r="G64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.79233053559997135</v>
       </c>
       <c r="H64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.8002525072907033</v>
       </c>
       <c r="I64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.6402020058325627</v>
       </c>
       <c r="J64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.6402020058325627</v>
       </c>
       <c r="K64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.64660359911800269</v>
       </c>
       <c r="L64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.56666395191692154</v>
       </c>
       <c r="M64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.6936112241268938</v>
       </c>
       <c r="N64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.70748680560495047</v>
       </c>
       <c r="O64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.72164213670958088</v>
       </c>
       <c r="P64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.73605856746568032</v>
       </c>
       <c r="Q64" s="7">
-        <f t="shared" si="104"/>
+        <f t="shared" si="118"/>
         <v>0.75079204779856312</v>
       </c>
     </row>
@@ -4158,63 +4152,63 @@
         <v>48507</v>
       </c>
       <c r="C65">
-        <f t="shared" ref="C65:Q65" si="105">(C$8*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <f t="shared" ref="C65:Q65" si="119">(C$8*(1+C$21+C$26+C$27+C$28))*C$33</f>
         <v>49839</v>
       </c>
       <c r="D65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>50586</v>
       </c>
       <c r="E65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>45080.735294117643</v>
       </c>
       <c r="F65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>38318.624999999993</v>
       </c>
       <c r="G65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>38318.624999999993</v>
       </c>
       <c r="H65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>38702.249999999993</v>
       </c>
       <c r="I65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>30961.8</v>
       </c>
       <c r="J65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>30961.8</v>
       </c>
       <c r="K65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>31271.399999999998</v>
       </c>
       <c r="L65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>30289.343999999997</v>
       </c>
       <c r="M65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>37074.031199999998</v>
       </c>
       <c r="N65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>37815.794999999998</v>
       </c>
       <c r="O65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>38571.717599999996</v>
       </c>
       <c r="P65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>39343.372199999998</v>
       </c>
       <c r="Q65">
-        <f t="shared" si="105"/>
+        <f t="shared" si="119"/>
         <v>40129.972199999997</v>
       </c>
     </row>
@@ -4227,63 +4221,63 @@
         <v>1</v>
       </c>
       <c r="C66" s="7">
-        <f t="shared" ref="C66:Q66" si="106">C65/$B65</f>
+        <f t="shared" ref="C66:Q66" si="120">C65/$B65</f>
         <v>1.0274599542334095</v>
       </c>
       <c r="D66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>1.0428597934318757</v>
       </c>
       <c r="E66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.92936556155024308</v>
       </c>
       <c r="F66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.78996072731770661</v>
       </c>
       <c r="G66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.78996072731770661</v>
       </c>
       <c r="H66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.79786937967715987</v>
       </c>
       <c r="I66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.63829550374172794</v>
       </c>
       <c r="J66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.63829550374172794</v>
       </c>
       <c r="K66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.64467808769868262</v>
       </c>
       <c r="L66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.6244324324324324</v>
       </c>
       <c r="M66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.76430270270270262</v>
       </c>
       <c r="N66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.77959459459459457</v>
       </c>
       <c r="O66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.79517837837837835</v>
       </c>
       <c r="P66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.8110864864864864</v>
       </c>
       <c r="Q66" s="7">
-        <f t="shared" si="106"/>
+        <f t="shared" si="120"/>
         <v>0.82730270270270267</v>
       </c>
     </row>
@@ -4296,63 +4290,63 @@
         <v>56119.5</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:Q67" si="107">(C$11*(1+C$21+C$26+C$27+C$28))*C$33</f>
+        <f t="shared" ref="C67:Q67" si="121">(C$11*(1+C$21+C$26+C$27+C$28))*C$33</f>
         <v>57504</v>
       </c>
       <c r="D67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>58366.5</v>
       </c>
       <c r="E67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>52014.70588235293</v>
       </c>
       <c r="F67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>44212.499999999993</v>
       </c>
       <c r="G67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>44212.499999999993</v>
       </c>
       <c r="H67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>44654.624999999993</v>
       </c>
       <c r="I67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>35723.699999999997</v>
       </c>
       <c r="J67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>35723.699999999997</v>
       </c>
       <c r="K67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>36081</v>
       </c>
       <c r="L67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>30289.343999999997</v>
       </c>
       <c r="M67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>37074.031199999998</v>
       </c>
       <c r="N67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>37815.794999999998</v>
       </c>
       <c r="O67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>38571.717599999996</v>
       </c>
       <c r="P67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>41750.368199999997</v>
       </c>
       <c r="Q67">
-        <f t="shared" si="107"/>
+        <f t="shared" si="121"/>
         <v>45935.866799999996</v>
       </c>
     </row>
@@ -4365,67 +4359,79 @@
         <v>1</v>
       </c>
       <c r="C68" s="7">
-        <f t="shared" ref="C68:Q68" si="108">C67/$B67</f>
+        <f t="shared" ref="C68:Q68" si="122">C67/$B67</f>
         <v>1.0246705690535376</v>
       </c>
       <c r="D68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>1.0400395584422526</v>
       </c>
       <c r="E68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.92685618871074993</v>
       </c>
       <c r="F68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.78782776040413749</v>
       </c>
       <c r="G68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.78782776040413749</v>
       </c>
       <c r="H68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.79570603800817885</v>
       </c>
       <c r="I68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.6365648304065431</v>
       </c>
       <c r="J68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.6365648304065431</v>
       </c>
       <c r="K68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.64293160131505089</v>
       </c>
       <c r="L68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.53972939887204974</v>
       </c>
       <c r="M68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.66062654157645739</v>
       </c>
       <c r="N68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.67384411835458258</v>
       </c>
       <c r="O68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.68731399246251301</v>
       </c>
       <c r="P68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.74395474300376874</v>
       </c>
       <c r="Q68" s="7">
-        <f t="shared" si="108"/>
+        <f t="shared" si="122"/>
         <v>0.81853663699783485</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A46:Q46">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A38:XFD38">
     <cfRule type="colorScale" priority="15">
       <colorScale>
@@ -4464,18 +4470,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:XFD44">
     <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A46:Q46">
-    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4619,60 +4613,60 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="13">
         <v>2007</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="13">
         <v>2008</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="13">
         <v>2009</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="13">
         <v>2010</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="13">
         <v>2011</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="13">
         <v>2012</v>
       </c>
-      <c r="H1" s="14">
+      <c r="H1" s="13">
         <v>2013</v>
       </c>
-      <c r="I1" s="14">
+      <c r="I1" s="13">
         <v>2014</v>
       </c>
-      <c r="J1" s="14">
+      <c r="J1" s="13">
         <v>2015</v>
       </c>
-      <c r="K1" s="14">
+      <c r="K1" s="13">
         <v>2016</v>
       </c>
-      <c r="L1" s="14">
+      <c r="L1" s="13">
         <v>2017</v>
       </c>
-      <c r="M1" s="14">
+      <c r="M1" s="13">
         <v>2018</v>
       </c>
-      <c r="N1" s="14">
+      <c r="N1" s="13">
         <v>2019</v>
       </c>
-      <c r="O1" s="14">
+      <c r="O1" s="13">
         <v>2020</v>
       </c>
-      <c r="P1" s="14">
+      <c r="P1" s="13">
         <v>2021</v>
       </c>
-      <c r="Q1" s="14">
+      <c r="Q1" s="13">
         <v>2022</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -4705,27 +4699,27 @@
       <c r="K2">
         <v>22862</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2">
         <v>26614</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2">
         <v>27146</v>
       </c>
-      <c r="N2" s="13">
+      <c r="N2">
         <v>27689</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2">
         <v>28243</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2">
         <v>28808</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2">
         <v>29384</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -4758,27 +4752,27 @@
       <c r="K3">
         <v>28357</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3">
         <v>30805</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3">
         <v>31422</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3">
         <v>32050</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3">
         <v>32691</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3">
         <v>33345</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3">
         <v>34012</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -4811,27 +4805,27 @@
       <c r="K4">
         <v>30302</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4">
         <v>36461</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4">
         <v>37191</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4">
         <v>37935</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4">
         <v>38694</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4">
         <v>39467</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4">
         <v>40257</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -4864,27 +4858,27 @@
       <c r="K5">
         <v>32156</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5">
         <v>36461</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5">
         <v>37191</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5">
         <v>37935</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5">
         <v>38694</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5">
         <v>39467</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5">
         <v>40257</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -4917,27 +4911,27 @@
       <c r="K6">
         <v>34746</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="14">
         <v>46208</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="14">
         <v>47132</v>
       </c>
-      <c r="N6" s="15">
+      <c r="N6" s="14">
         <v>48075</v>
       </c>
-      <c r="O6" s="15">
+      <c r="O6" s="14">
         <v>49036</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="14">
         <v>50017</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="14">
         <v>51017</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B7">
@@ -4970,27 +4964,27 @@
       <c r="K7">
         <v>36312</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="14">
         <v>46208</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="14">
         <v>47132</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="14">
         <v>48075</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="14">
         <v>49036</v>
       </c>
-      <c r="P7" s="15">
+      <c r="P7" s="14">
         <v>50017</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="14">
         <v>51017</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -5023,27 +5017,27 @@
       <c r="K8">
         <v>38200</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="14">
         <v>46208</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="14">
         <v>47132</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N8" s="14">
         <v>48075</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O8" s="14">
         <v>49036</v>
       </c>
-      <c r="P8" s="15">
+      <c r="P8" s="14">
         <v>50017</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="14">
         <v>51017</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -5076,27 +5070,27 @@
       <c r="K9">
         <v>40090</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="14">
         <v>46208</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="14">
         <v>47132</v>
       </c>
-      <c r="N9" s="15">
+      <c r="N9" s="14">
         <v>48075</v>
       </c>
-      <c r="O9" s="15">
+      <c r="O9" s="14">
         <v>49036</v>
       </c>
-      <c r="P9" s="15">
+      <c r="P9" s="14">
         <v>53077</v>
       </c>
-      <c r="Q9" s="15">
+      <c r="Q9" s="14">
         <v>58398</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B10">
@@ -5129,27 +5123,27 @@
       <c r="K10">
         <v>41979</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="14">
         <v>46208</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="14">
         <v>47132</v>
       </c>
-      <c r="N10" s="15">
+      <c r="N10" s="14">
         <v>48075</v>
       </c>
-      <c r="O10" s="15">
+      <c r="O10" s="14">
         <v>49036</v>
       </c>
-      <c r="P10" s="15">
+      <c r="P10" s="14">
         <v>53077</v>
       </c>
-      <c r="Q10" s="15">
+      <c r="Q10" s="14">
         <v>58398</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -5182,22 +5176,22 @@
       <c r="K11">
         <v>43868</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="14">
         <v>46208</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="14">
         <v>47132</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="14">
         <v>48075</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="14">
         <v>49036</v>
       </c>
-      <c r="P11" s="15">
+      <c r="P11" s="14">
         <v>53077</v>
       </c>
-      <c r="Q11" s="15">
+      <c r="Q11" s="14">
         <v>58398</v>
       </c>
     </row>
@@ -5220,60 +5214,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="13">
         <v>2007</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="13">
         <v>2008</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="13">
         <v>2009</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="13">
         <v>2010</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="13">
         <v>2011</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="13">
         <v>2012</v>
       </c>
-      <c r="H1" s="14">
+      <c r="H1" s="13">
         <v>2013</v>
       </c>
-      <c r="I1" s="14">
+      <c r="I1" s="13">
         <v>2014</v>
       </c>
-      <c r="J1" s="14">
+      <c r="J1" s="13">
         <v>2015</v>
       </c>
-      <c r="K1" s="14">
+      <c r="K1" s="13">
         <v>2016</v>
       </c>
-      <c r="L1" s="14">
+      <c r="L1" s="13">
         <v>2017</v>
       </c>
-      <c r="M1" s="14">
+      <c r="M1" s="13">
         <v>2018</v>
       </c>
-      <c r="N1" s="14">
+      <c r="N1" s="13">
         <v>2019</v>
       </c>
-      <c r="O1" s="14">
+      <c r="O1" s="13">
         <v>2020</v>
       </c>
-      <c r="P1" s="14">
+      <c r="P1" s="13">
         <v>2021</v>
       </c>
-      <c r="Q1" s="14">
+      <c r="Q1" s="13">
         <v>2022</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B2">
@@ -5306,27 +5300,27 @@
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="15">
         <v>2130</v>
       </c>
-      <c r="M2" s="16">
+      <c r="M2" s="15">
         <v>2172</v>
       </c>
-      <c r="N2" s="16">
+      <c r="N2" s="15">
         <v>2216</v>
       </c>
-      <c r="O2" s="16">
+      <c r="O2" s="15">
         <v>2260</v>
       </c>
-      <c r="P2" s="16">
+      <c r="P2" s="15">
         <v>2305</v>
       </c>
-      <c r="Q2" s="16">
+      <c r="Q2" s="15">
         <v>2351</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>53</v>
       </c>
       <c r="B3">
@@ -5359,27 +5353,27 @@
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="15">
         <v>2465</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="15">
         <v>2514</v>
       </c>
-      <c r="N3" s="16">
+      <c r="N3" s="15">
         <v>2564</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="15">
         <v>2616</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="15">
         <v>2668</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="15">
         <v>2721</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>54</v>
       </c>
       <c r="B4">
@@ -5412,27 +5406,27 @@
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="15">
         <v>2917</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="15">
         <v>2976</v>
       </c>
-      <c r="N4" s="16">
+      <c r="N4" s="15">
         <v>3035</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="15">
         <v>3096</v>
       </c>
-      <c r="P4" s="15">
+      <c r="P4" s="14">
         <v>3158</v>
       </c>
-      <c r="Q4" s="15">
+      <c r="Q4" s="14">
         <v>3221</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>55</v>
       </c>
       <c r="B5">
@@ -5465,27 +5459,27 @@
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="15">
         <v>3697</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="15">
         <v>3771</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="15">
         <v>3846</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5" s="15">
         <v>3923</v>
       </c>
-      <c r="P5" s="15">
+      <c r="P5" s="14">
         <v>4002</v>
       </c>
-      <c r="Q5" s="15">
+      <c r="Q5" s="14">
         <v>4082</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>56</v>
       </c>
       <c r="B6">
@@ -5518,22 +5512,22 @@
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="15">
         <v>3697</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="15">
         <v>3771</v>
       </c>
-      <c r="N6" s="16">
+      <c r="N6" s="15">
         <v>3846</v>
       </c>
-      <c r="O6" s="16">
+      <c r="O6" s="15">
         <v>3923</v>
       </c>
-      <c r="P6" s="15">
+      <c r="P6" s="14">
         <v>4247</v>
       </c>
-      <c r="Q6" s="15">
+      <c r="Q6" s="14">
         <v>4672</v>
       </c>
     </row>
@@ -5544,10 +5538,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC320418-4F28-FA43-96AE-D726FA4ADFA3}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5556,60 +5550,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="14">
+      <c r="B1" s="13">
         <v>2007</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="13">
         <v>2008</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="13">
         <v>2009</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="13">
         <v>2010</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="13">
         <v>2011</v>
       </c>
-      <c r="G1" s="14">
+      <c r="G1" s="13">
         <v>2012</v>
       </c>
-      <c r="H1" s="14">
+      <c r="H1" s="13">
         <v>2013</v>
       </c>
-      <c r="I1" s="14">
+      <c r="I1" s="13">
         <v>2014</v>
       </c>
-      <c r="J1" s="14">
+      <c r="J1" s="13">
         <v>2015</v>
       </c>
-      <c r="K1" s="14">
+      <c r="K1" s="13">
         <v>2016</v>
       </c>
-      <c r="L1" s="14">
+      <c r="L1" s="13">
         <v>2017</v>
       </c>
-      <c r="M1" s="14">
+      <c r="M1" s="13">
         <v>2018</v>
       </c>
-      <c r="N1" s="14">
+      <c r="N1" s="13">
         <v>2019</v>
       </c>
-      <c r="O1" s="14">
+      <c r="O1" s="13">
         <v>2020</v>
       </c>
-      <c r="P1" s="14">
+      <c r="P1" s="13">
         <v>2021</v>
       </c>
-      <c r="Q1" s="14">
+      <c r="Q1" s="13">
         <v>2022</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B2">
@@ -5662,7 +5656,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="6">
@@ -5715,7 +5709,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="6">
@@ -5768,142 +5762,243 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="16">
+        <v>83.3</v>
+      </c>
+      <c r="C5" s="16">
+        <v>86.2</v>
+      </c>
+      <c r="D5" s="16">
+        <v>87.9</v>
+      </c>
+      <c r="E5" s="16">
+        <v>90.1</v>
+      </c>
+      <c r="F5" s="16">
+        <v>93.6</v>
+      </c>
+      <c r="G5" s="16">
+        <v>96</v>
+      </c>
+      <c r="H5" s="16">
+        <v>98.2</v>
+      </c>
+      <c r="I5" s="16">
+        <v>99.6</v>
+      </c>
+      <c r="J5" s="16">
+        <v>100</v>
+      </c>
+      <c r="K5" s="16">
+        <v>101</v>
+      </c>
+      <c r="L5" s="16">
+        <v>103.6</v>
+      </c>
+      <c r="M5" s="16">
+        <v>106</v>
+      </c>
+      <c r="N5" s="16">
+        <v>107.8</v>
+      </c>
+      <c r="O5" s="16">
+        <v>108.9</v>
+      </c>
+      <c r="P5" s="16">
+        <v>111.6</v>
+      </c>
+      <c r="Q5" s="16">
+        <v>120.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f>$B$3/B3</f>
         <v>1</v>
       </c>
-      <c r="C5">
-        <f t="shared" ref="C5:Q5" si="0">$B$3/C3</f>
+      <c r="C6">
+        <f t="shared" ref="C6:Q6" si="0">$B$3/C3</f>
         <v>0.96576151121605658</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>0.94457274826789839</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>0.91498881431767332</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <f t="shared" si="0"/>
         <v>0.87580299785867233</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>0.85119667013527578</v>
       </c>
-      <c r="H5">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>0.8304568527918782</v>
       </c>
-      <c r="I5">
+      <c r="I6">
         <f t="shared" si="0"/>
         <v>0.81799999999999995</v>
       </c>
-      <c r="J5">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>0.81799999999999995</v>
       </c>
-      <c r="K5">
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>0.81231380337636538</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <f t="shared" si="0"/>
         <v>0.79110251450676972</v>
       </c>
-      <c r="M5">
+      <c r="M6">
         <f t="shared" si="0"/>
         <v>0.77242681775259669</v>
       </c>
-      <c r="N5">
+      <c r="N6">
         <f t="shared" si="0"/>
         <v>0.75881261595547311</v>
       </c>
-      <c r="O5">
+      <c r="O6">
         <f t="shared" si="0"/>
         <v>0.75252989880404775</v>
       </c>
-      <c r="P5">
+      <c r="P6">
         <f t="shared" si="0"/>
         <v>0.73297491039426521</v>
       </c>
-      <c r="Q5">
+      <c r="Q6">
         <f t="shared" si="0"/>
         <v>0.67214461791290059</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f>$B$4/B4</f>
         <v>1</v>
       </c>
-      <c r="C6">
-        <f t="shared" ref="C6:Q6" si="1">$B$4/C4</f>
+      <c r="C7">
+        <f t="shared" ref="C7:Q7" si="1">$B$4/C4</f>
         <v>0.96182495344506513</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <f t="shared" si="1"/>
         <v>0.96677585400093591</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <f t="shared" si="1"/>
         <v>0.92397137745974955</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <f t="shared" si="1"/>
         <v>0.87840136054421769</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <f t="shared" si="1"/>
         <v>0.85125669550885874</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <f t="shared" si="1"/>
         <v>0.82606957217113153</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <f t="shared" si="1"/>
         <v>0.80703124999999998</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <f t="shared" si="1"/>
         <v>0.79922630560928432</v>
       </c>
-      <c r="K6">
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>0.78525275560623331</v>
       </c>
-      <c r="L6">
+      <c r="L7">
         <f t="shared" si="1"/>
         <v>0.75816513761467885</v>
       </c>
-      <c r="M6">
+      <c r="M7">
         <f t="shared" si="1"/>
         <v>0.7336647727272726</v>
       </c>
-      <c r="N6">
+      <c r="N7">
         <f t="shared" si="1"/>
         <v>0.71537396121883656</v>
       </c>
-      <c r="O6">
+      <c r="O7">
         <f t="shared" si="1"/>
         <v>0.70487888092801088</v>
       </c>
-      <c r="P6">
+      <c r="P7">
         <f t="shared" si="1"/>
         <v>0.67737704918032782</v>
       </c>
-      <c r="Q6">
+      <c r="Q7">
         <f t="shared" si="1"/>
         <v>0.6071113723185424</v>
       </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="16"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="16"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="16"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="16"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="16"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5912,7 +6007,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BC5F88-8D8D-784C-8D83-41F1D70B721C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
@@ -5948,7 +6043,6 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added data on MPs' base pay since 2010; NB this reflects only base pay not total remuneration, work done, additional declared financial interests which may be enabled through holding elected office, etc, etc.
</commit_message>
<xml_diff>
--- a/Pay 2007-2022.xlsx
+++ b/Pay 2007-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelshaw/fpr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D3C7D1-FAFC-9941-B86A-C0A65B42E555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DCDA61-1D74-A540-AAED-FF7DB700D482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13140" yWindow="0" windowWidth="20460" windowHeight="21000" activeTab="3" xr2:uid="{E1BF444D-A2ED-614E-ACCD-35609FC30102}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
   <si>
     <t>FY1</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>CPIH</t>
+  </si>
+  <si>
+    <t>CPIH Multiplier</t>
   </si>
 </sst>
 </file>
@@ -5538,10 +5541,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC320418-4F28-FA43-96AE-D726FA4ADFA3}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5816,144 +5819,279 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6">
+        <f>$B$2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:Q6" si="0">$B$2/C2</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.88235294117647045</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f>$B$3/B3</f>
         <v>1</v>
       </c>
-      <c r="C6">
-        <f t="shared" ref="C6:Q6" si="0">$B$3/C3</f>
+      <c r="C7">
+        <f t="shared" ref="C7:Q7" si="1">$B$3/C3</f>
         <v>0.96576151121605658</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+      <c r="D7">
+        <f t="shared" si="1"/>
         <v>0.94457274826789839</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="E7">
+        <f t="shared" si="1"/>
         <v>0.91498881431767332</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
+      <c r="F7">
+        <f t="shared" si="1"/>
         <v>0.87580299785867233</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
+      <c r="G7">
+        <f t="shared" si="1"/>
         <v>0.85119667013527578</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
+      <c r="H7">
+        <f t="shared" si="1"/>
         <v>0.8304568527918782</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
+      <c r="I7">
+        <f t="shared" si="1"/>
         <v>0.81799999999999995</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
+      <c r="J7">
+        <f t="shared" si="1"/>
         <v>0.81799999999999995</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
+      <c r="K7">
+        <f t="shared" si="1"/>
         <v>0.81231380337636538</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
+      <c r="L7">
+        <f t="shared" si="1"/>
         <v>0.79110251450676972</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
+      <c r="M7">
+        <f t="shared" si="1"/>
         <v>0.77242681775259669</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
+      <c r="N7">
+        <f t="shared" si="1"/>
         <v>0.75881261595547311</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="0"/>
+      <c r="O7">
+        <f t="shared" si="1"/>
         <v>0.75252989880404775</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
+      <c r="P7">
+        <f t="shared" si="1"/>
         <v>0.73297491039426521</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="0"/>
+      <c r="Q7">
+        <f t="shared" si="1"/>
         <v>0.67214461791290059</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <f>$B$4/B4</f>
         <v>1</v>
       </c>
-      <c r="C7">
-        <f t="shared" ref="C7:Q7" si="1">$B$4/C4</f>
+      <c r="C8">
+        <f t="shared" ref="C8:Q8" si="2">$B$4/C4</f>
         <v>0.96182495344506513</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
+      <c r="D8">
+        <f t="shared" si="2"/>
         <v>0.96677585400093591</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
+      <c r="E8">
+        <f t="shared" si="2"/>
         <v>0.92397137745974955</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
+      <c r="F8">
+        <f t="shared" si="2"/>
         <v>0.87840136054421769</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
+      <c r="G8">
+        <f t="shared" si="2"/>
         <v>0.85125669550885874</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
+      <c r="H8">
+        <f t="shared" si="2"/>
         <v>0.82606957217113153</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
+      <c r="I8">
+        <f t="shared" si="2"/>
         <v>0.80703124999999998</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="1"/>
+      <c r="J8">
+        <f t="shared" si="2"/>
         <v>0.79922630560928432</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
+      <c r="K8">
+        <f t="shared" si="2"/>
         <v>0.78525275560623331</v>
       </c>
-      <c r="L7">
-        <f t="shared" si="1"/>
+      <c r="L8">
+        <f t="shared" si="2"/>
         <v>0.75816513761467885</v>
       </c>
-      <c r="M7">
-        <f t="shared" si="1"/>
+      <c r="M8">
+        <f t="shared" si="2"/>
         <v>0.7336647727272726</v>
       </c>
-      <c r="N7">
-        <f t="shared" si="1"/>
+      <c r="N8">
+        <f t="shared" si="2"/>
         <v>0.71537396121883656</v>
       </c>
-      <c r="O7">
-        <f t="shared" si="1"/>
+      <c r="O8">
+        <f t="shared" si="2"/>
         <v>0.70487888092801088</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="1"/>
+      <c r="P8">
+        <f t="shared" si="2"/>
         <v>0.67737704918032782</v>
       </c>
-      <c r="Q7">
-        <f t="shared" si="1"/>
+      <c r="Q8">
+        <f t="shared" si="2"/>
         <v>0.6071113723185424</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D13" s="16"/>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9">
+        <f>$B$5/B5</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:Q9" si="3">$B$5/C5</f>
+        <v>0.96635730858468671</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="3"/>
+        <v>0.94766780432309439</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>0.92452830188679247</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>0.88995726495726502</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0.8677083333333333</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>0.84826883910386963</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>0.83634538152610449</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>0.82475247524752471</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>0.80405405405405406</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>0.78584905660377358</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>0.76492194674012848</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>0.74641577060931896</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>0.6912863070539419</v>
+      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D14" s="16"/>
@@ -5999,6 +6137,9 @@
     </row>
     <row r="28" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D28" s="16"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>